<commit_message>
Added Use Cases specifications to excel
</commit_message>
<xml_diff>
--- a/projeto/Especificação de Use Cases.XLSX
+++ b/projeto/Especificação de Use Cases.XLSX
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7B7561-514C-49D3-AE01-06B912827AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C477EC9-CD17-4B38-8B4B-AC19E9BCC34A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Use Case:</t>
   </si>
@@ -95,6 +95,63 @@
   </si>
   <si>
     <t>3 &lt;&lt;extends&gt;&gt; Confecionar receita</t>
+  </si>
+  <si>
+    <t>Gerar lista de ingredientes</t>
+  </si>
+  <si>
+    <t>1. Decide  gerar a lista de ingredientes</t>
+  </si>
+  <si>
+    <t>2. Consulta ementa semanal do ator</t>
+  </si>
+  <si>
+    <t>3. Calcula os ingredientes necessários para a semana</t>
+  </si>
+  <si>
+    <t>4. Mostra os ingredientes e as respetivas quantidades</t>
+  </si>
+  <si>
+    <t>5. Confirma a lista de ingredientes.</t>
+  </si>
+  <si>
+    <t>6.  &lt;&lt;extends&gt;&gt; aceder a serviços externos</t>
+  </si>
+  <si>
+    <t>5.2 Adiciona ingrediente à lista</t>
+  </si>
+  <si>
+    <t>5.3 Volta ao passo 5</t>
+  </si>
+  <si>
+    <t>Comportamento Alternativo 2[Ator quer remover ingredientes à lista](passo 5)</t>
+  </si>
+  <si>
+    <t>Comportamento Alternativo 1[Ator quer adicionar ingrediente à lista](passo 5)</t>
+  </si>
+  <si>
+    <t>5.2 Remove ingrediente da lista</t>
+  </si>
+  <si>
+    <t>5.1 Escolhe o ingrediente e quantidade a adicionar</t>
+  </si>
+  <si>
+    <t>5.1 Escolhe o ingrediente e quantidade a remover</t>
+  </si>
+  <si>
+    <t>5.2.1 Indica que o ingrediente não existe na lista</t>
+  </si>
+  <si>
+    <t>5.2.2 Volta ao passo 5</t>
+  </si>
+  <si>
+    <t>Comportamento Alternativo 3 [Quantidade do ingrediente é zero](passo 5.2)</t>
+  </si>
+  <si>
+    <t>6. Guarda a lista de ingredientes</t>
+  </si>
+  <si>
+    <t>Lista de ingredientes guardada no sistema</t>
   </si>
 </sst>
 </file>
@@ -220,48 +277,97 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:J15"/>
+  <dimension ref="C4:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,181 +663,397 @@
     <col min="8" max="8" width="21.28515625" customWidth="1"/>
     <col min="9" max="9" width="21.140625" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="10"/>
       <c r="H4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="10"/>
+      <c r="M4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="10"/>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="10"/>
       <c r="H5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="10"/>
+      <c r="M5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="10"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="10"/>
       <c r="H6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="3:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="7" t="s">
+      <c r="J6" s="10"/>
+      <c r="M6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-      <c r="D8" s="4" t="s">
+      <c r="M7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="11"/>
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="10" t="s">
+      <c r="E8" s="3"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
+      <c r="J8" s="3"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="11"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="14" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="7"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
+      <c r="M9" s="11"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="11"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="14"/>
-    </row>
-    <row r="11" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="7"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="32"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="11"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="8" t="s">
+      <c r="H11" s="11"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="32"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="21"/>
+    </row>
+    <row r="12" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="14" t="s">
+      <c r="E12" s="3"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
+      <c r="J12" s="17"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="20"/>
+    </row>
+    <row r="13" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="14"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="6"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="18"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="15"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C15" s="9" t="s">
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="23"/>
+    </row>
+    <row r="15" spans="3:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="15"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="9"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="24"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M16" s="11"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M17" s="11"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="23"/>
+    </row>
+    <row r="18" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M18" s="11"/>
+      <c r="N18" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="O18" s="25"/>
+    </row>
+    <row r="19" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M19" s="11"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="25"/>
+    </row>
+    <row r="20" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M20" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O20" s="27"/>
+    </row>
+    <row r="21" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M21" s="29"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="28"/>
+    </row>
+    <row r="22" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M22" s="29"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M23" s="29"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="23"/>
+    </row>
+    <row r="24" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M24" s="29"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M25" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O25" s="27"/>
+    </row>
+    <row r="26" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M26" s="29"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="28"/>
+    </row>
+    <row r="27" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M27" s="29"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="13:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M28" s="29"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="23"/>
+    </row>
+    <row r="29" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M29" s="29"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M30" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M31" s="29"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+    </row>
+    <row r="32" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M32" s="29"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+    </row>
+    <row r="33" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M33" s="29"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M34" s="29"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="38">
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="M30:M34"/>
+    <mergeCell ref="M25:M29"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="M20:M24"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="M7:M19"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="I12:I13"/>
     <mergeCell ref="H7:H13"/>
     <mergeCell ref="C7:C11"/>
     <mergeCell ref="C12:C14"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J12:J13"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="N10:N12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="N13:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Editar ementa semanal + added favoritos and confecionados to class diagram
</commit_message>
<xml_diff>
--- a/projeto/Especificação de Use Cases.XLSX
+++ b/projeto/Especificação de Use Cases.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CésarAugustodaCostaB\Documents\Projects\LI4\projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2145777-7D16-4C16-B1FB-EAC8733899B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E000BEE1-BF24-4EBE-9F17-B82F26EBDE10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="157">
   <si>
     <t>Use Case:</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Pós-condição:</t>
   </si>
   <si>
-    <t>Encontrou mais que uma receita</t>
-  </si>
-  <si>
     <t>Receita foi consultada</t>
   </si>
   <si>
@@ -439,6 +436,66 @@
   </si>
   <si>
     <t>Exceção 2[Utilizador cancela Confecionar receita](em qualquer passo)</t>
+  </si>
+  <si>
+    <t>Editar ementa semanal</t>
+  </si>
+  <si>
+    <t>Ementa semanal foi alterada</t>
+  </si>
+  <si>
+    <t>1. Mostra todas as receitas na ementa nos dias e refeições já escolhidas</t>
+  </si>
+  <si>
+    <t>2. Escolhe uma receita</t>
+  </si>
+  <si>
+    <t>3. Escolhe uma refeição e dia da semana</t>
+  </si>
+  <si>
+    <t>4. Escolhe adicionar uma receita à ementa</t>
+  </si>
+  <si>
+    <t>5. Verifica escolhas</t>
+  </si>
+  <si>
+    <t>6. Adiciona receita à ementa</t>
+  </si>
+  <si>
+    <t>Encontrou pelo menos uma receita</t>
+  </si>
+  <si>
+    <t>Comportamento Alternativo 1 [Escolhe remover uma receita] (passo 4)</t>
+  </si>
+  <si>
+    <t>4.1 Escolhe remover uma receita da ementa</t>
+  </si>
+  <si>
+    <t>4.2 Verifica escolhas</t>
+  </si>
+  <si>
+    <t>4.2 Remove receita da ementa</t>
+  </si>
+  <si>
+    <t>Comportamento Alternativo 2 [Já existe receita para aquela refeição e dia] (passo 5)</t>
+  </si>
+  <si>
+    <t>5.1 Indica que já existe uma receita</t>
+  </si>
+  <si>
+    <t>5.2 Pergunta se quer substituir receita</t>
+  </si>
+  <si>
+    <t>5.3 Confirma</t>
+  </si>
+  <si>
+    <t>5.4 Remove receita antiga</t>
+  </si>
+  <si>
+    <t>5.5 volta ao passo 6</t>
+  </si>
+  <si>
+    <t>Exceção 1 [Não confirma](Passo 5.3)</t>
   </si>
 </sst>
 </file>
@@ -462,7 +519,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +566,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor rgb="FFBDD7EE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -585,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -626,127 +689,161 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1133,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J106" sqref="J106"/>
+    <sheetView tabSelected="1" topLeftCell="E69" zoomScale="101" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H88" sqref="H88:H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1243,7 @@
     <col min="6" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" customWidth="1"/>
     <col min="9" max="9" width="21.140625" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" customWidth="1"/>
     <col min="12" max="12" width="8.5703125" customWidth="1"/>
     <col min="13" max="13" width="20.85546875" customWidth="1"/>
@@ -1159,466 +1256,466 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="27"/>
       <c r="H4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="23"/>
+      <c r="J4" s="27"/>
       <c r="M4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="23"/>
+      <c r="O4" s="27"/>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="27"/>
       <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="23"/>
+      <c r="J5" s="27"/>
       <c r="M5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="23"/>
+      <c r="O5" s="27"/>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="23"/>
+      <c r="D6" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="27"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="23"/>
+      <c r="I6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="27"/>
       <c r="M6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="N6" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="27"/>
+    </row>
+    <row r="7" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="23"/>
-    </row>
-    <row r="7" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="29" t="s">
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="H7" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="40"/>
+      <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="29"/>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="3"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="O8" s="3"/>
     </row>
     <row r="9" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="29"/>
+      <c r="C9" s="40"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="40"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="29"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="29"/>
+      <c r="M9" s="40"/>
       <c r="N9" s="3"/>
       <c r="O9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="29"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="40"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="42"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="45"/>
+      <c r="O10" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="31"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="33" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="29"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="40"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="42"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="44"/>
+    </row>
+    <row r="12" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="31"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="33"/>
-    </row>
-    <row r="12" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="22" t="s">
+      <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="18"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="33"/>
+      <c r="J12" s="45"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="44"/>
     </row>
     <row r="13" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="22"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="40"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="45"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="18"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="33" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="22"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="33"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="44"/>
     </row>
     <row r="15" spans="3:15" ht="45" x14ac:dyDescent="0.25">
       <c r="C15" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="6"/>
       <c r="J15" s="9"/>
-      <c r="M15" s="29"/>
+      <c r="M15" s="40"/>
       <c r="N15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="10"/>
+    </row>
+    <row r="16" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M16" s="40"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="O15" s="10"/>
-    </row>
-    <row r="16" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M16" s="29"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="33" t="s">
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M17" s="40"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="44"/>
+    </row>
+    <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="40"/>
+      <c r="N18" s="44" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M17" s="29"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="33"/>
-    </row>
-    <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M18" s="29"/>
-      <c r="N18" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="O18" s="34"/>
+      <c r="O18" s="46"/>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M19" s="29"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="34"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="46"/>
     </row>
     <row r="20" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="23"/>
+      <c r="D20" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="27"/>
       <c r="H20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="27"/>
+      <c r="M20" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="23"/>
-      <c r="M20" s="22" t="s">
+      <c r="N20" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="N20" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="O20" s="32"/>
+      <c r="O20" s="43"/>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="23"/>
+      <c r="E21" s="27"/>
       <c r="H21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="23" t="s">
+      <c r="I21" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="23"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="32"/>
+      <c r="J21" s="27"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="43"/>
     </row>
     <row r="22" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="23"/>
+      <c r="D22" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="27"/>
       <c r="H22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="23" t="s">
+      <c r="I22" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="27"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="J22" s="23"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="33" t="s">
+    </row>
+    <row r="23" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M23" s="26"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="44"/>
+    </row>
+    <row r="24" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C24" s="36"/>
+      <c r="D24" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M23" s="22"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="33"/>
-    </row>
-    <row r="24" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C24" s="30"/>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="10"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="J24" s="3"/>
-      <c r="M24" s="22"/>
+      <c r="M24" s="26"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="30"/>
+      <c r="C25" s="36"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="36"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="39" t="s">
+      <c r="M25" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="M25" s="22" t="s">
+      <c r="N25" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="N25" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="O25" s="32"/>
+      <c r="O25" s="43"/>
     </row>
     <row r="26" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="30"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="H26" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="H26" s="36"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="M26" s="22"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="32"/>
+        <v>48</v>
+      </c>
+      <c r="M26" s="26"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="43"/>
     </row>
     <row r="27" spans="3:15" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="8"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="40"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="19"/>
       <c r="J27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M27" s="26"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="M27" s="22"/>
-      <c r="N27" s="32"/>
-      <c r="O27" s="33" t="s">
+    </row>
+    <row r="28" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="37" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H28" s="36" t="s">
+      <c r="I28" s="38"/>
+      <c r="J28" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="I28" s="37"/>
-      <c r="J28" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="M28" s="22"/>
-      <c r="N28" s="32"/>
-      <c r="O28" s="33"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="44"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H29" s="36"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="38"/>
-      <c r="M29" s="22"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="39"/>
+      <c r="M29" s="26"/>
       <c r="N29" s="11"/>
       <c r="O29" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="38"/>
-      <c r="M30" s="22" t="s">
+      <c r="H30" s="37"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="39"/>
+      <c r="M30" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="N30" s="45"/>
+      <c r="O30" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H31" s="36"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="38"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="39"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="38"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="39"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M33" s="22"/>
+      <c r="M33" s="26"/>
       <c r="N33" s="10"/>
       <c r="O33" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="23"/>
-      <c r="M34" s="22"/>
+      <c r="D34" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="27"/>
+      <c r="M34" s="26"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
     </row>
@@ -1626,233 +1723,233 @@
       <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="D35" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="23"/>
+      <c r="E35" s="27"/>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="D36" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="27"/>
+    </row>
+    <row r="37" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C38" s="36"/>
+      <c r="D38" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="23"/>
-    </row>
-    <row r="37" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C38" s="30"/>
-      <c r="D38" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C39" s="30"/>
+      <c r="C39" s="36"/>
       <c r="D39" s="10"/>
       <c r="E39" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C40" s="30"/>
+      <c r="C40" s="36"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C41" s="36"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C41" s="30"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="3" t="s">
+    <row r="42" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="37" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="42" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="36" t="s">
+      <c r="D42" s="38"/>
+      <c r="E42" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="37"/>
-      <c r="E42" s="38" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="36"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="38"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="39"/>
       <c r="H43" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I43" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J43" s="23"/>
+      <c r="I43" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="J43" s="27"/>
       <c r="M43" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N43" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="O43" s="23"/>
+      <c r="N43" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="O43" s="27"/>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="36"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="38"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="39"/>
       <c r="H44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I44" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="J44" s="23"/>
+      <c r="I44" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J44" s="27"/>
       <c r="M44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N44" s="23" t="s">
+      <c r="N44" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="O44" s="23"/>
+      <c r="O44" s="27"/>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="36"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="38"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="39"/>
       <c r="H45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I45" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="J45" s="23"/>
+      <c r="I45" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="J45" s="27"/>
       <c r="M45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N45" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="O45" s="23"/>
+      <c r="N45" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="O45" s="27"/>
     </row>
     <row r="46" spans="3:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="36"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="38"/>
-      <c r="H46" s="29" t="s">
+      <c r="C46" s="37"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="39"/>
+      <c r="H46" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="J46" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J46" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M46" s="21" t="s">
+      <c r="M46" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="N46" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N46" s="2" t="s">
+      <c r="O46" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O46" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="47" spans="3:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="H47" s="29"/>
+      <c r="H47" s="40"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="M47" s="33"/>
+      <c r="N47" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="M47" s="21"/>
-      <c r="N47" s="13" t="s">
+      <c r="O47" s="13"/>
+    </row>
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H48" s="40"/>
+      <c r="I48" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="O47" s="13"/>
-    </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H48" s="29"/>
-      <c r="I48" s="13" t="s">
-        <v>72</v>
-      </c>
       <c r="J48" s="13"/>
-      <c r="M48" s="21"/>
+      <c r="M48" s="33"/>
       <c r="N48" s="13"/>
       <c r="O48" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H49" s="29"/>
+      <c r="H49" s="40"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="M49" s="21"/>
+        <v>73</v>
+      </c>
+      <c r="M49" s="33"/>
       <c r="N49" s="13"/>
       <c r="O49" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H50" s="29"/>
+      <c r="H50" s="40"/>
       <c r="I50" s="13"/>
       <c r="J50" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M50" s="26" t="s">
         <v>76</v>
-      </c>
-      <c r="M50" s="22" t="s">
-        <v>77</v>
       </c>
       <c r="N50" s="13"/>
       <c r="O50" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D51" s="23" t="s">
+      <c r="D51" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="27"/>
+      <c r="H51" s="26" t="s">
         <v>79</v>
-      </c>
-      <c r="E51" s="23"/>
-      <c r="H51" s="22" t="s">
-        <v>80</v>
       </c>
       <c r="I51" s="13"/>
       <c r="J51" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="M51" s="22"/>
+        <v>80</v>
+      </c>
+      <c r="M51" s="26"/>
       <c r="N51" s="13"/>
       <c r="O51" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C52" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="23" t="s">
+      <c r="D52" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="23"/>
-      <c r="H52" s="22"/>
+      <c r="E52" s="27"/>
+      <c r="H52" s="26"/>
       <c r="I52" s="13"/>
       <c r="J52" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="M52" s="22"/>
+        <v>82</v>
+      </c>
+      <c r="M52" s="26"/>
       <c r="N52" s="13"/>
       <c r="O52" s="13"/>
     </row>
@@ -1860,480 +1957,642 @@
       <c r="C53" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53" s="23"/>
-      <c r="H53" s="22"/>
+      <c r="D53" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" s="27"/>
+      <c r="H53" s="26"/>
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
-      <c r="M53" s="28" t="s">
-        <v>85</v>
+      <c r="M53" s="35" t="s">
+        <v>84</v>
       </c>
       <c r="N53" s="13"/>
       <c r="O53" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M54" s="28"/>
+      <c r="M54" s="35"/>
       <c r="N54" s="13"/>
       <c r="O54" s="13"/>
     </row>
     <row r="55" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C55" s="21"/>
+      <c r="C55" s="33"/>
       <c r="D55" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E55" s="13"/>
-      <c r="M55" s="28"/>
+      <c r="M55" s="35"/>
       <c r="N55" s="13"/>
       <c r="O55" s="13"/>
     </row>
     <row r="56" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="21"/>
+      <c r="C56" s="33"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="M56" s="41" t="s">
         <v>88</v>
-      </c>
-      <c r="M56" s="26" t="s">
-        <v>89</v>
       </c>
       <c r="N56" s="13"/>
       <c r="O56" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C57" s="33"/>
+      <c r="D57" s="13" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C57" s="21"/>
-      <c r="D57" s="13" t="s">
-        <v>91</v>
-      </c>
       <c r="E57" s="10"/>
-      <c r="M57" s="26"/>
+      <c r="M57" s="41"/>
       <c r="N57" s="13"/>
       <c r="O57" s="13"/>
     </row>
-    <row r="58" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="27" t="s">
+    <row r="58" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D58" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D58" s="13" t="s">
-        <v>93</v>
-      </c>
       <c r="E58" s="13"/>
+      <c r="H58" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I58" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="J58" s="27"/>
     </row>
     <row r="59" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C59" s="27"/>
+      <c r="C59" s="34"/>
       <c r="D59" s="13"/>
       <c r="E59" s="13" t="s">
-        <v>94</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I59" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J59" s="27"/>
     </row>
     <row r="60" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C60" s="27"/>
+      <c r="C60" s="34"/>
       <c r="D60" s="13"/>
       <c r="E60" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="61" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C61" s="27"/>
+        <v>94</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I60" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="J60" s="27"/>
+    </row>
+    <row r="61" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="34"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H61" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="35" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="62" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C62" s="28" t="s">
+      <c r="D62" s="13"/>
+      <c r="E62" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C63" s="28"/>
+      <c r="H62" s="40"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="3:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="35"/>
       <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
+      <c r="E63" s="29"/>
+      <c r="H63" s="40"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="31"/>
     </row>
     <row r="64" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C64" s="28"/>
+      <c r="C64" s="35"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
-    </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H64" s="40"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="31"/>
+    </row>
+    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H65" s="40"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="32"/>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H66" s="40"/>
+      <c r="I66" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J66" s="13"/>
+    </row>
+    <row r="67" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H67" s="40"/>
+      <c r="I67" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="J67" s="28"/>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H68" s="40"/>
+      <c r="I68" s="31"/>
+      <c r="J68" s="62"/>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C69" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D69" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="E69" s="23"/>
-    </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D69" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E69" s="27"/>
+      <c r="H69" s="40"/>
+      <c r="I69" s="32"/>
+      <c r="J69" s="29"/>
+    </row>
+    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C70" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="23" t="s">
+      <c r="D70" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E70" s="23"/>
-    </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E70" s="27"/>
+      <c r="H70" s="40"/>
+      <c r="I70" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="J70" s="13"/>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C71" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D71" s="23" t="s">
+      <c r="D71" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E71" s="27"/>
+      <c r="H71" s="40"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="13"/>
+    </row>
+    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C72" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72" s="40"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="3:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="40"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="E71" s="23"/>
-    </row>
-    <row r="72" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C72" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="73" spans="3:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C73" s="29"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24" t="s">
+      <c r="H73" s="40"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C74" s="40"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
+      <c r="H74" s="40"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="23"/>
+    </row>
+    <row r="75" spans="3:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="40"/>
+      <c r="D75" s="15" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="74" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C74" s="29"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-    </row>
-    <row r="75" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C75" s="29"/>
-      <c r="D75" s="15" t="s">
+      <c r="E75" s="11"/>
+      <c r="H75" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="I75" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="J75" s="21"/>
+    </row>
+    <row r="76" spans="3:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="40"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="E75" s="11"/>
-    </row>
-    <row r="76" spans="3:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="29"/>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24" t="s">
+      <c r="H76" s="26"/>
+      <c r="I76" s="66"/>
+      <c r="J76" s="21"/>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C77" s="40"/>
+      <c r="D77" s="32"/>
+      <c r="E77" s="32"/>
+      <c r="H77" s="26"/>
+      <c r="I77" s="65"/>
+      <c r="J77" s="21"/>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C78" s="40"/>
+      <c r="D78" s="15" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="77" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C77" s="29"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-    </row>
-    <row r="78" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C78" s="29"/>
-      <c r="D78" s="15" t="s">
-        <v>104</v>
-      </c>
       <c r="E78" s="15"/>
-    </row>
-    <row r="79" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="29"/>
+      <c r="H78" s="26"/>
+      <c r="I78" s="63"/>
+      <c r="J78" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="79" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="40"/>
       <c r="D79" s="15"/>
       <c r="E79" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H79" s="26"/>
+      <c r="I79" s="28"/>
+      <c r="J79" s="23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C80" s="40"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="23" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="80" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C80" s="29"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="17" t="s">
+      <c r="H80" s="26"/>
+      <c r="I80" s="29"/>
+      <c r="J80" s="23"/>
+    </row>
+    <row r="81" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C81" s="40"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="23"/>
+      <c r="H81" s="68" t="s">
+        <v>150</v>
+      </c>
+      <c r="I81" s="10"/>
+      <c r="J81" s="23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="82" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C82" s="40"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="23"/>
+      <c r="H82" s="68"/>
+      <c r="I82" s="10"/>
+      <c r="J82" s="23"/>
+    </row>
+    <row r="83" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C83" s="40"/>
+      <c r="D83" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I80" s="16"/>
-    </row>
-    <row r="81" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C81" s="29"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="17"/>
-    </row>
-    <row r="82" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C82" s="29"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="17"/>
-    </row>
-    <row r="83" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C83" s="29"/>
-      <c r="D83" s="17" t="s">
+      <c r="E83" s="24"/>
+      <c r="H83" s="68"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C84" s="40"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="25"/>
+      <c r="H84" s="68"/>
+      <c r="I84" s="10"/>
+      <c r="J84" s="52"/>
+    </row>
+    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C85" s="40"/>
+      <c r="D85" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E83" s="44"/>
-    </row>
-    <row r="84" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C84" s="29"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="45"/>
-    </row>
-    <row r="85" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C85" s="29"/>
-      <c r="D85" s="11" t="s">
-        <v>108</v>
-      </c>
       <c r="E85" s="11"/>
-    </row>
-    <row r="86" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C86" s="29"/>
+      <c r="H85" s="68"/>
+      <c r="I85" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="J85" s="10"/>
+    </row>
+    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C86" s="40"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="87" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C87" s="29"/>
+        <v>108</v>
+      </c>
+      <c r="H86" s="68"/>
+      <c r="I86" s="10"/>
+      <c r="J86" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C87" s="40"/>
       <c r="D87" s="10"/>
       <c r="E87" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="88" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C88" s="29"/>
+        <v>116</v>
+      </c>
+      <c r="H87" s="68"/>
+      <c r="I87" s="10"/>
+      <c r="J87" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C88" s="40"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H88" s="69" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C89" s="40"/>
+      <c r="D89" s="48"/>
+      <c r="E89" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="H88" s="16"/>
-    </row>
-    <row r="89" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C89" s="29"/>
-      <c r="D89" s="47"/>
-      <c r="E89" s="17" t="s">
+      <c r="H89" s="70"/>
+    </row>
+    <row r="90" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C90" s="40"/>
+      <c r="D90" s="49"/>
+      <c r="E90" s="23"/>
+      <c r="H90" s="70"/>
+    </row>
+    <row r="91" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C91" s="40"/>
+      <c r="D91" s="11" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="90" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C90" s="29"/>
-      <c r="D90" s="48"/>
-      <c r="E90" s="17"/>
-    </row>
-    <row r="91" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C91" s="29"/>
-      <c r="D91" s="11" t="s">
-        <v>123</v>
-      </c>
       <c r="E91" s="11"/>
-    </row>
-    <row r="92" spans="3:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C92" s="29"/>
+      <c r="H91" s="70"/>
+    </row>
+    <row r="92" spans="3:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C92" s="40"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H92" s="70"/>
+    </row>
+    <row r="93" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C93" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D93" s="20"/>
+      <c r="E93" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="94" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C94" s="26"/>
+      <c r="D94" s="20"/>
+      <c r="E94" s="21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="95" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C95" s="26"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="21"/>
+    </row>
+    <row r="96" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C96" s="26"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="21"/>
+    </row>
+    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C97" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D97" s="20"/>
+      <c r="E97" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="98" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C98" s="26"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="99" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C99" s="26"/>
+      <c r="D99" s="20"/>
+      <c r="E99" s="21"/>
+    </row>
+    <row r="100" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C100" s="26"/>
+      <c r="D100" s="20"/>
+      <c r="E100" s="21"/>
+    </row>
+    <row r="101" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C101" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="D101" s="48"/>
+      <c r="E101" s="50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="102" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C102" s="47"/>
+      <c r="D102" s="49"/>
+      <c r="E102" s="51"/>
+    </row>
+    <row r="103" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C103" s="47"/>
+      <c r="D103" s="20"/>
+      <c r="E103" s="21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="104" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C104" s="47"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="105" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C105" s="55" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="93" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C93" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D93" s="42"/>
-      <c r="E93" s="46" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="94" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C94" s="22"/>
-      <c r="D94" s="42"/>
-      <c r="E94" s="46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="95" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C95" s="22"/>
-      <c r="D95" s="42"/>
-      <c r="E95" s="46"/>
-    </row>
-    <row r="96" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C96" s="22"/>
-      <c r="D96" s="42"/>
-      <c r="E96" s="46"/>
-    </row>
-    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C97" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="D97" s="42"/>
-      <c r="E97" s="46" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="98" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C98" s="22"/>
-      <c r="D98" s="42"/>
-      <c r="E98" s="46" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="99" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C99" s="22"/>
-      <c r="D99" s="42"/>
-      <c r="E99" s="46"/>
-    </row>
-    <row r="100" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C100" s="22"/>
-      <c r="D100" s="42"/>
-      <c r="E100" s="46"/>
-    </row>
-    <row r="101" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C101" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="D101" s="47"/>
-      <c r="E101" s="51" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="102" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C102" s="49"/>
-      <c r="D102" s="48"/>
-      <c r="E102" s="52"/>
-    </row>
-    <row r="103" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C103" s="49"/>
-      <c r="D103" s="42"/>
-      <c r="E103" s="46" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="104" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C104" s="49"/>
-      <c r="D104" s="42"/>
-      <c r="E104" s="46" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="105" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C105" s="54" t="s">
+      <c r="D105" s="20"/>
+      <c r="E105" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="D105" s="42"/>
-      <c r="E105" s="53" t="s">
+    </row>
+    <row r="106" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C106" s="56"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="22"/>
+      <c r="J106" s="16"/>
+    </row>
+    <row r="107" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C107" s="57"/>
+      <c r="D107" s="20"/>
+      <c r="E107" s="21"/>
+    </row>
+    <row r="108" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C108" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="D108" s="58" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="106" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C106" s="55"/>
-      <c r="D106" s="42"/>
-      <c r="E106" s="53"/>
-      <c r="J106" s="16"/>
-    </row>
-    <row r="107" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C107" s="56"/>
-      <c r="D107" s="42"/>
-      <c r="E107" s="46"/>
-    </row>
-    <row r="108" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C108" s="54" t="s">
-        <v>132</v>
-      </c>
-      <c r="D108" s="41" t="s">
+      <c r="E108" s="59"/>
+    </row>
+    <row r="109" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C109" s="56"/>
+      <c r="D109" s="58"/>
+      <c r="E109" s="59"/>
+    </row>
+    <row r="110" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C110" s="56"/>
+      <c r="D110" s="20"/>
+      <c r="E110" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="E108" s="50"/>
-    </row>
-    <row r="109" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C109" s="55"/>
-      <c r="D109" s="41"/>
-      <c r="E109" s="50"/>
-    </row>
-    <row r="110" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C110" s="55"/>
-      <c r="D110" s="42"/>
-      <c r="E110" s="46" t="s">
+    </row>
+    <row r="111" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C111" s="56"/>
+      <c r="D111" s="60"/>
+      <c r="E111" s="52" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="111" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C111" s="55"/>
-      <c r="D111" s="19"/>
-      <c r="E111" s="43" t="s">
+    <row r="112" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C112" s="56"/>
+      <c r="D112" s="61"/>
+      <c r="E112" s="52"/>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C113" s="56"/>
+      <c r="D113" s="10" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="112" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C112" s="55"/>
-      <c r="D112" s="20"/>
-      <c r="E112" s="43"/>
-    </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C113" s="55"/>
-      <c r="D113" s="10" t="s">
-        <v>130</v>
-      </c>
       <c r="E113" s="10"/>
     </row>
     <row r="114" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C114" s="56"/>
+      <c r="C114" s="57"/>
       <c r="D114" s="10"/>
       <c r="E114" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="115" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C115" s="28" t="s">
-        <v>133</v>
+      <c r="C115" s="35" t="s">
+        <v>132</v>
       </c>
       <c r="D115" s="13"/>
-      <c r="E115" s="43" t="s">
-        <v>136</v>
+      <c r="E115" s="52" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="116" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C116" s="28"/>
+      <c r="C116" s="35"/>
       <c r="D116" s="13"/>
-      <c r="E116" s="43"/>
+      <c r="E116" s="52"/>
     </row>
     <row r="117" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C117" s="28"/>
+      <c r="C117" s="35"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="118" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C118" s="57" t="s">
-        <v>137</v>
+      <c r="C118" s="53" t="s">
+        <v>136</v>
       </c>
       <c r="D118" s="13"/>
       <c r="E118" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="119" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C119" s="58"/>
+      <c r="C119" s="54"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
     <row r="120" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C120" s="58"/>
+      <c r="C120" s="54"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
     <row r="121" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C121" s="58"/>
+      <c r="C121" s="54"/>
       <c r="D121" s="10"/>
       <c r="E121" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="101">
+  <mergeCells count="119">
+    <mergeCell ref="H88:H92"/>
+    <mergeCell ref="H61:H74"/>
+    <mergeCell ref="I75:I77"/>
+    <mergeCell ref="J79:J80"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="H75:H80"/>
+    <mergeCell ref="J81:J82"/>
+    <mergeCell ref="J83:J84"/>
+    <mergeCell ref="H81:H87"/>
     <mergeCell ref="C115:C117"/>
     <mergeCell ref="E115:E116"/>
     <mergeCell ref="C118:C121"/>
@@ -2421,6 +2680,16 @@
     <mergeCell ref="M53:M55"/>
     <mergeCell ref="C54:C57"/>
     <mergeCell ref="M56:M57"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="C93:C96"/>
+    <mergeCell ref="E80:E82"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="J62:J65"/>
     <mergeCell ref="C58:C61"/>
     <mergeCell ref="C62:C64"/>
     <mergeCell ref="D69:E69"/>
@@ -2430,11 +2699,10 @@
     <mergeCell ref="E76:E77"/>
     <mergeCell ref="D73:D74"/>
     <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="C93:C96"/>
-    <mergeCell ref="E80:E82"/>
+    <mergeCell ref="I67:I69"/>
+    <mergeCell ref="J67:J69"/>
+    <mergeCell ref="I70:I71"/>
+    <mergeCell ref="J73:J74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added Editar Ementa semanal to sequence diagram
</commit_message>
<xml_diff>
--- a/projeto/Especificação de Use Cases.XLSX
+++ b/projeto/Especificação de Use Cases.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CésarAugustodaCostaB\Documents\Projects\LI4\projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E000BEE1-BF24-4EBE-9F17-B82F26EBDE10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39E8628-1B40-495D-88D0-28CDA9B93DAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="158">
   <si>
     <t>Use Case:</t>
   </si>
@@ -492,10 +492,13 @@
     <t>5.4 Remove receita antiga</t>
   </si>
   <si>
-    <t>5.5 volta ao passo 6</t>
-  </si>
-  <si>
     <t>Exceção 1 [Não confirma](Passo 5.3)</t>
+  </si>
+  <si>
+    <t>5.5 Volta ao passo 6</t>
+  </si>
+  <si>
+    <t>5.3.1 Termina editar ementa semanal</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,6 +574,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -705,7 +714,119 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -713,18 +834,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -734,116 +843,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1230,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E69" zoomScale="101" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88:H92"/>
+    <sheetView tabSelected="1" topLeftCell="E67" zoomScale="101" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M80" sqref="M80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,73 +1265,73 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="50"/>
       <c r="H4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="27"/>
+      <c r="J4" s="50"/>
       <c r="M4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="27"/>
+      <c r="O4" s="50"/>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="50"/>
       <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="27"/>
+      <c r="J5" s="50"/>
       <c r="M5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="27" t="s">
+      <c r="N5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="27"/>
+      <c r="O5" s="50"/>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="27"/>
+      <c r="E6" s="50"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="27"/>
+      <c r="J6" s="50"/>
       <c r="M6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="27" t="s">
+      <c r="N6" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="27"/>
+      <c r="O6" s="50"/>
     </row>
     <row r="7" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="25" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1331,7 +1340,7 @@
       <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="25" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1340,7 +1349,7 @@
       <c r="J7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="40" t="s">
+      <c r="M7" s="25" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="2" t="s">
@@ -1351,101 +1360,101 @@
       </c>
     </row>
     <row r="8" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="40"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="H8" s="40"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="M8" s="40"/>
+      <c r="M8" s="25"/>
       <c r="N8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="O8" s="3"/>
     </row>
     <row r="9" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="40"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="42" t="s">
+      <c r="H9" s="25"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="40"/>
+      <c r="M9" s="25"/>
       <c r="N9" s="3"/>
       <c r="O9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="40"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="42"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="44" t="s">
+      <c r="H10" s="25"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="52"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="53" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="40"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="40"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="42"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="44"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="52"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="53"/>
     </row>
     <row r="12" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="32" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="42" t="s">
+      <c r="H12" s="25"/>
+      <c r="I12" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="45"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="44"/>
+      <c r="J12" s="51"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="53"/>
     </row>
     <row r="13" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="26"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="40"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="45"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="44" t="s">
+      <c r="H13" s="25"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="51"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="53" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="26"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
         <v>27</v>
@@ -1453,9 +1462,9 @@
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="44"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="53"/>
     </row>
     <row r="15" spans="3:15" ht="45" x14ac:dyDescent="0.25">
       <c r="C15" s="7" t="s">
@@ -1468,101 +1477,101 @@
       <c r="H15" s="8"/>
       <c r="I15" s="6"/>
       <c r="J15" s="9"/>
-      <c r="M15" s="40"/>
+      <c r="M15" s="25"/>
       <c r="N15" s="4" t="s">
         <v>30</v>
       </c>
       <c r="O15" s="10"/>
     </row>
     <row r="16" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M16" s="40"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="44" t="s">
+      <c r="M16" s="25"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="53" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M17" s="40"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="44"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="53"/>
     </row>
     <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M18" s="40"/>
-      <c r="N18" s="44" t="s">
+      <c r="M18" s="25"/>
+      <c r="N18" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="O18" s="46"/>
+      <c r="O18" s="54"/>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M19" s="40"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="46"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="54"/>
     </row>
     <row r="20" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="27"/>
+      <c r="E20" s="50"/>
       <c r="H20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="27"/>
-      <c r="M20" s="26" t="s">
+      <c r="J20" s="50"/>
+      <c r="M20" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="N20" s="42" t="s">
+      <c r="N20" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="O20" s="43"/>
+      <c r="O20" s="55"/>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="27"/>
+      <c r="E21" s="50"/>
       <c r="H21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="27"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="43"/>
+      <c r="J21" s="50"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="55"/>
     </row>
     <row r="22" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="27"/>
+      <c r="E22" s="50"/>
       <c r="H22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="27" t="s">
+      <c r="I22" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="J22" s="27"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="44" t="s">
+      <c r="J22" s="50"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="53" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="56" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1571,7 +1580,7 @@
       <c r="E23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="36" t="s">
+      <c r="H23" s="56" t="s">
         <v>10</v>
       </c>
       <c r="I23" s="2" t="s">
@@ -1580,128 +1589,128 @@
       <c r="J23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="26"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="44"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="53"/>
     </row>
     <row r="24" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C24" s="36"/>
+      <c r="C24" s="56"/>
       <c r="D24" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="H24" s="36"/>
+      <c r="H24" s="56"/>
       <c r="I24" s="3" t="s">
         <v>41</v>
       </c>
       <c r="J24" s="3"/>
-      <c r="M24" s="26"/>
+      <c r="M24" s="32"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="36"/>
+      <c r="C25" s="56"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="36"/>
+      <c r="H25" s="56"/>
       <c r="I25" s="10"/>
       <c r="J25" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="M25" s="26" t="s">
+      <c r="M25" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="42" t="s">
+      <c r="N25" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="O25" s="43"/>
+      <c r="O25" s="55"/>
     </row>
     <row r="26" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="36"/>
+      <c r="C26" s="56"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H26" s="36"/>
+      <c r="H26" s="56"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="M26" s="26"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="43"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="52"/>
+      <c r="O26" s="55"/>
     </row>
     <row r="27" spans="3:15" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="8"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="H27" s="36"/>
+      <c r="H27" s="56"/>
       <c r="I27" s="19"/>
       <c r="J27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M27" s="26"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="44" t="s">
+      <c r="M27" s="32"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="53" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H28" s="37" t="s">
+      <c r="H28" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="I28" s="38"/>
-      <c r="J28" s="39" t="s">
+      <c r="I28" s="58"/>
+      <c r="J28" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="M28" s="26"/>
-      <c r="N28" s="43"/>
-      <c r="O28" s="44"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="53"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H29" s="37"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="39"/>
-      <c r="M29" s="26"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="59"/>
+      <c r="M29" s="32"/>
       <c r="N29" s="11"/>
       <c r="O29" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H30" s="37"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="39"/>
-      <c r="M30" s="26" t="s">
+      <c r="H30" s="57"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="59"/>
+      <c r="M30" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45" t="s">
+      <c r="N30" s="51"/>
+      <c r="O30" s="51" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H31" s="37"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="39"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="59"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="51"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H32" s="37"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="39"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="59"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="51"/>
+      <c r="O32" s="51"/>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M33" s="26"/>
+      <c r="M33" s="32"/>
       <c r="N33" s="10"/>
       <c r="O33" s="10" t="s">
         <v>55</v>
@@ -1711,11 +1720,11 @@
       <c r="C34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="27" t="s">
+      <c r="D34" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="M34" s="26"/>
+      <c r="E34" s="50"/>
+      <c r="M34" s="32"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
     </row>
@@ -1723,22 +1732,22 @@
       <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="27"/>
+      <c r="E35" s="50"/>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="27"/>
+      <c r="E36" s="50"/>
     </row>
     <row r="37" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="56" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -1749,104 +1758,104 @@
       </c>
     </row>
     <row r="38" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C38" s="36"/>
+      <c r="C38" s="56"/>
       <c r="D38" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C39" s="36"/>
+      <c r="C39" s="56"/>
       <c r="D39" s="10"/>
       <c r="E39" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C40" s="36"/>
+      <c r="C40" s="56"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="41" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C41" s="36"/>
+      <c r="C41" s="56"/>
       <c r="D41" s="17"/>
       <c r="E41" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="42" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="38"/>
-      <c r="E42" s="39" t="s">
+      <c r="D42" s="58"/>
+      <c r="E42" s="59" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="37"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="39"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="59"/>
       <c r="H43" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I43" s="27" t="s">
+      <c r="I43" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="J43" s="27"/>
+      <c r="J43" s="50"/>
       <c r="M43" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N43" s="27" t="s">
+      <c r="N43" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="O43" s="27"/>
+      <c r="O43" s="50"/>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="37"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="39"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="59"/>
       <c r="H44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I44" s="27" t="s">
+      <c r="I44" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="J44" s="27"/>
+      <c r="J44" s="50"/>
       <c r="M44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N44" s="27" t="s">
+      <c r="N44" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="O44" s="27"/>
+      <c r="O44" s="50"/>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="37"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="39"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="59"/>
       <c r="H45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I45" s="27" t="s">
+      <c r="I45" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="J45" s="27"/>
+      <c r="J45" s="50"/>
       <c r="M45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N45" s="27" t="s">
+      <c r="N45" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="O45" s="27"/>
+      <c r="O45" s="50"/>
     </row>
     <row r="46" spans="3:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="37"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="39"/>
-      <c r="H46" s="40" t="s">
+      <c r="C46" s="57"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="59"/>
+      <c r="H46" s="25" t="s">
         <v>10</v>
       </c>
       <c r="I46" s="2" t="s">
@@ -1855,7 +1864,7 @@
       <c r="J46" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M46" s="33" t="s">
+      <c r="M46" s="60" t="s">
         <v>10</v>
       </c>
       <c r="N46" s="2" t="s">
@@ -1866,48 +1875,48 @@
       </c>
     </row>
     <row r="47" spans="3:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="H47" s="40"/>
+      <c r="H47" s="25"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="M47" s="33"/>
+      <c r="M47" s="60"/>
       <c r="N47" s="13" t="s">
         <v>70</v>
       </c>
       <c r="O47" s="13"/>
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H48" s="40"/>
+      <c r="H48" s="25"/>
       <c r="I48" s="13" t="s">
         <v>71</v>
       </c>
       <c r="J48" s="13"/>
-      <c r="M48" s="33"/>
+      <c r="M48" s="60"/>
       <c r="N48" s="13"/>
       <c r="O48" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="49" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H49" s="40"/>
+      <c r="H49" s="25"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="M49" s="33"/>
+      <c r="M49" s="60"/>
       <c r="N49" s="13"/>
       <c r="O49" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="50" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H50" s="40"/>
+      <c r="H50" s="25"/>
       <c r="I50" s="13"/>
       <c r="J50" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="M50" s="26" t="s">
+      <c r="M50" s="32" t="s">
         <v>76</v>
       </c>
       <c r="N50" s="13"/>
@@ -1919,18 +1928,18 @@
       <c r="C51" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D51" s="27" t="s">
+      <c r="D51" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="E51" s="27"/>
-      <c r="H51" s="26" t="s">
+      <c r="E51" s="50"/>
+      <c r="H51" s="32" t="s">
         <v>79</v>
       </c>
       <c r="I51" s="13"/>
       <c r="J51" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="M51" s="26"/>
+      <c r="M51" s="32"/>
       <c r="N51" s="13"/>
       <c r="O51" s="13" t="s">
         <v>81</v>
@@ -1940,16 +1949,16 @@
       <c r="C52" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="27" t="s">
+      <c r="D52" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="27"/>
-      <c r="H52" s="26"/>
+      <c r="E52" s="50"/>
+      <c r="H52" s="32"/>
       <c r="I52" s="13"/>
       <c r="J52" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="M52" s="26"/>
+      <c r="M52" s="32"/>
       <c r="N52" s="13"/>
       <c r="O52" s="13"/>
     </row>
@@ -1957,11 +1966,11 @@
       <c r="C53" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="27" t="s">
+      <c r="D53" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="E53" s="27"/>
-      <c r="H53" s="26"/>
+      <c r="E53" s="50"/>
+      <c r="H53" s="32"/>
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
       <c r="M53" s="35" t="s">
@@ -1973,7 +1982,7 @@
       </c>
     </row>
     <row r="54" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="33" t="s">
+      <c r="C54" s="60" t="s">
         <v>10</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -1987,7 +1996,7 @@
       <c r="O54" s="13"/>
     </row>
     <row r="55" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C55" s="33"/>
+      <c r="C55" s="60"/>
       <c r="D55" s="13" t="s">
         <v>86</v>
       </c>
@@ -1997,12 +2006,12 @@
       <c r="O55" s="13"/>
     </row>
     <row r="56" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="33"/>
+      <c r="C56" s="60"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="M56" s="41" t="s">
+      <c r="M56" s="61" t="s">
         <v>88</v>
       </c>
       <c r="N56" s="13"/>
@@ -2011,17 +2020,17 @@
       </c>
     </row>
     <row r="57" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C57" s="33"/>
+      <c r="C57" s="60"/>
       <c r="D57" s="13" t="s">
         <v>90</v>
       </c>
       <c r="E57" s="10"/>
-      <c r="M57" s="41"/>
+      <c r="M57" s="61"/>
       <c r="N57" s="13"/>
       <c r="O57" s="13"/>
     </row>
     <row r="58" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="34" t="s">
+      <c r="C58" s="67" t="s">
         <v>91</v>
       </c>
       <c r="D58" s="13" t="s">
@@ -2031,13 +2040,13 @@
       <c r="H58" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I58" s="27" t="s">
+      <c r="I58" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="J58" s="27"/>
+      <c r="J58" s="50"/>
     </row>
     <row r="59" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C59" s="34"/>
+      <c r="C59" s="67"/>
       <c r="D59" s="13"/>
       <c r="E59" s="13" t="s">
         <v>93</v>
@@ -2045,13 +2054,13 @@
       <c r="H59" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I59" s="27" t="s">
+      <c r="I59" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="J59" s="27"/>
+      <c r="J59" s="50"/>
     </row>
     <row r="60" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C60" s="34"/>
+      <c r="C60" s="67"/>
       <c r="D60" s="13"/>
       <c r="E60" s="13" t="s">
         <v>94</v>
@@ -2059,18 +2068,18 @@
       <c r="H60" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I60" s="27" t="s">
+      <c r="I60" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="J60" s="27"/>
+      <c r="J60" s="50"/>
     </row>
     <row r="61" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="34"/>
+      <c r="C61" s="67"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="H61" s="40" t="s">
+      <c r="H61" s="25" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="2" t="s">
@@ -2085,95 +2094,95 @@
         <v>96</v>
       </c>
       <c r="D62" s="13"/>
-      <c r="E62" s="28" t="s">
+      <c r="E62" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="H62" s="40"/>
+      <c r="H62" s="25"/>
       <c r="I62" s="13"/>
-      <c r="J62" s="30" t="s">
+      <c r="J62" s="64" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="63" spans="3:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C63" s="35"/>
       <c r="D63" s="13"/>
-      <c r="E63" s="29"/>
-      <c r="H63" s="40"/>
+      <c r="E63" s="31"/>
+      <c r="H63" s="25"/>
       <c r="I63" s="13"/>
-      <c r="J63" s="31"/>
+      <c r="J63" s="65"/>
     </row>
     <row r="64" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C64" s="35"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
-      <c r="H64" s="40"/>
+      <c r="H64" s="25"/>
       <c r="I64" s="13"/>
-      <c r="J64" s="31"/>
-    </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="H65" s="40"/>
+      <c r="J64" s="65"/>
+    </row>
+    <row r="65" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="H65" s="25"/>
       <c r="I65" s="13"/>
-      <c r="J65" s="32"/>
-    </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="H66" s="40"/>
+      <c r="J65" s="66"/>
+    </row>
+    <row r="66" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="H66" s="25"/>
       <c r="I66" s="13" t="s">
         <v>140</v>
       </c>
       <c r="J66" s="13"/>
     </row>
-    <row r="67" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H67" s="40"/>
-      <c r="I67" s="30" t="s">
+    <row r="67" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H67" s="25"/>
+      <c r="I67" s="64" t="s">
         <v>141</v>
       </c>
-      <c r="J67" s="28"/>
-    </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="H68" s="40"/>
-      <c r="I68" s="31"/>
-      <c r="J68" s="62"/>
-    </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J67" s="30"/>
+    </row>
+    <row r="68" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="H68" s="25"/>
+      <c r="I68" s="65"/>
+      <c r="J68" s="68"/>
+    </row>
+    <row r="69" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C69" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D69" s="27" t="s">
+      <c r="D69" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="E69" s="27"/>
-      <c r="H69" s="40"/>
-      <c r="I69" s="32"/>
-      <c r="J69" s="29"/>
-    </row>
-    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="E69" s="50"/>
+      <c r="H69" s="25"/>
+      <c r="I69" s="66"/>
+      <c r="J69" s="31"/>
+    </row>
+    <row r="70" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C70" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="27" t="s">
+      <c r="D70" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E70" s="27"/>
-      <c r="H70" s="40"/>
-      <c r="I70" s="28" t="s">
+      <c r="E70" s="50"/>
+      <c r="H70" s="25"/>
+      <c r="I70" s="30" t="s">
         <v>142</v>
       </c>
       <c r="J70" s="13"/>
     </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C71" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D71" s="27" t="s">
+      <c r="D71" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="E71" s="27"/>
-      <c r="H71" s="40"/>
-      <c r="I71" s="29"/>
+      <c r="E71" s="50"/>
+      <c r="H71" s="25"/>
+      <c r="I71" s="31"/>
       <c r="J71" s="13"/>
     </row>
-    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C72" s="40" t="s">
+    <row r="72" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C72" s="25" t="s">
         <v>10</v>
       </c>
       <c r="D72" s="2" t="s">
@@ -2182,216 +2191,223 @@
       <c r="E72" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H72" s="40"/>
+      <c r="H72" s="25"/>
       <c r="I72" s="10"/>
       <c r="J72" s="10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="3:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C73" s="40"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30" t="s">
+    <row r="73" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="25"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="H73" s="40"/>
+      <c r="H73" s="25"/>
       <c r="I73" s="10"/>
-      <c r="J73" s="23" t="s">
+      <c r="J73" s="29" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C74" s="40"/>
-      <c r="D74" s="32"/>
-      <c r="E74" s="32"/>
-      <c r="H74" s="40"/>
+    <row r="74" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C74" s="25"/>
+      <c r="D74" s="66"/>
+      <c r="E74" s="66"/>
+      <c r="H74" s="25"/>
       <c r="I74" s="10"/>
-      <c r="J74" s="23"/>
-    </row>
-    <row r="75" spans="3:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="40"/>
+      <c r="J74" s="29"/>
+    </row>
+    <row r="75" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="25"/>
       <c r="D75" s="15" t="s">
         <v>101</v>
       </c>
       <c r="E75" s="11"/>
-      <c r="H75" s="26" t="s">
+      <c r="H75" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="I75" s="64" t="s">
+      <c r="I75" s="26" t="s">
         <v>147</v>
       </c>
       <c r="J75" s="21"/>
     </row>
-    <row r="76" spans="3:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="40"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30" t="s">
+    <row r="76" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="25"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="H76" s="26"/>
-      <c r="I76" s="66"/>
+      <c r="H76" s="32"/>
+      <c r="I76" s="27"/>
       <c r="J76" s="21"/>
     </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C77" s="40"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32"/>
-      <c r="H77" s="26"/>
-      <c r="I77" s="65"/>
+    <row r="77" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C77" s="25"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="66"/>
+      <c r="H77" s="32"/>
+      <c r="I77" s="28"/>
       <c r="J77" s="21"/>
     </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C78" s="40"/>
+    <row r="78" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C78" s="25"/>
       <c r="D78" s="15" t="s">
         <v>103</v>
       </c>
       <c r="E78" s="15"/>
-      <c r="H78" s="26"/>
-      <c r="I78" s="63"/>
+      <c r="H78" s="32"/>
+      <c r="I78" s="23"/>
       <c r="J78" s="21" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="79" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="40"/>
+    <row r="79" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="25"/>
       <c r="D79" s="15"/>
       <c r="E79" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="H79" s="26"/>
-      <c r="I79" s="28"/>
-      <c r="J79" s="23" t="s">
+      <c r="H79" s="32"/>
+      <c r="I79" s="30"/>
+      <c r="J79" s="29" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C80" s="40"/>
+    <row r="80" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C80" s="25"/>
       <c r="D80" s="15"/>
-      <c r="E80" s="23" t="s">
+      <c r="E80" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="H80" s="26"/>
-      <c r="I80" s="29"/>
-      <c r="J80" s="23"/>
+      <c r="H80" s="32"/>
+      <c r="I80" s="31"/>
+      <c r="J80" s="29"/>
+      <c r="M80" s="16"/>
     </row>
     <row r="81" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C81" s="40"/>
+      <c r="C81" s="25"/>
       <c r="D81" s="15"/>
-      <c r="E81" s="23"/>
-      <c r="H81" s="68" t="s">
+      <c r="E81" s="29"/>
+      <c r="H81" s="34" t="s">
         <v>150</v>
       </c>
       <c r="I81" s="10"/>
-      <c r="J81" s="23" t="s">
+      <c r="J81" s="29" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="82" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C82" s="40"/>
+      <c r="C82" s="25"/>
       <c r="D82" s="15"/>
-      <c r="E82" s="23"/>
-      <c r="H82" s="68"/>
+      <c r="E82" s="29"/>
+      <c r="H82" s="34"/>
       <c r="I82" s="10"/>
-      <c r="J82" s="23"/>
+      <c r="J82" s="29"/>
     </row>
     <row r="83" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C83" s="40"/>
-      <c r="D83" s="23" t="s">
+      <c r="C83" s="25"/>
+      <c r="D83" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="E83" s="24"/>
-      <c r="H83" s="68"/>
+      <c r="E83" s="62"/>
+      <c r="H83" s="34"/>
       <c r="I83" s="10"/>
-      <c r="J83" s="52" t="s">
+      <c r="J83" s="33" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="84" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C84" s="40"/>
-      <c r="D84" s="23"/>
-      <c r="E84" s="25"/>
-      <c r="H84" s="68"/>
+      <c r="C84" s="25"/>
+      <c r="D84" s="29"/>
+      <c r="E84" s="63"/>
+      <c r="H84" s="34"/>
       <c r="I84" s="10"/>
-      <c r="J84" s="52"/>
+      <c r="J84" s="33"/>
     </row>
     <row r="85" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C85" s="40"/>
+      <c r="C85" s="25"/>
       <c r="D85" s="11" t="s">
         <v>107</v>
       </c>
       <c r="E85" s="11"/>
-      <c r="H85" s="68"/>
+      <c r="H85" s="34"/>
       <c r="I85" s="10" t="s">
         <v>153</v>
       </c>
       <c r="J85" s="10"/>
     </row>
     <row r="86" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C86" s="40"/>
+      <c r="C86" s="25"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H86" s="68"/>
+      <c r="H86" s="34"/>
       <c r="I86" s="10"/>
-      <c r="J86" s="67" t="s">
+      <c r="J86" s="24" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="87" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C87" s="40"/>
+      <c r="C87" s="25"/>
       <c r="D87" s="10"/>
       <c r="E87" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="H87" s="68"/>
+      <c r="H87" s="34"/>
       <c r="I87" s="10"/>
       <c r="J87" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C88" s="40"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="88" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C88" s="25"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="H88" s="69" t="s">
-        <v>156</v>
+      <c r="H88" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="I88" s="43"/>
+      <c r="J88" s="29" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="40"/>
-      <c r="D89" s="48"/>
-      <c r="E89" s="23" t="s">
+      <c r="C89" s="25"/>
+      <c r="D89" s="46"/>
+      <c r="E89" s="29" t="s">
         <v>121</v>
       </c>
       <c r="H89" s="70"/>
+      <c r="I89" s="44"/>
+      <c r="J89" s="29"/>
     </row>
     <row r="90" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C90" s="40"/>
-      <c r="D90" s="49"/>
-      <c r="E90" s="23"/>
-      <c r="H90" s="70"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="47"/>
+      <c r="E90" s="29"/>
+      <c r="H90" s="69"/>
     </row>
     <row r="91" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C91" s="40"/>
+      <c r="C91" s="25"/>
       <c r="D91" s="11" t="s">
         <v>122</v>
       </c>
       <c r="E91" s="11"/>
-      <c r="H91" s="70"/>
+      <c r="H91" s="69"/>
     </row>
     <row r="92" spans="3:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C92" s="40"/>
+      <c r="C92" s="25"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="H92" s="70"/>
+      <c r="H92" s="69"/>
     </row>
     <row r="93" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C93" s="26" t="s">
+      <c r="C93" s="32" t="s">
         <v>119</v>
       </c>
       <c r="D93" s="20"/>
@@ -2400,24 +2416,24 @@
       </c>
     </row>
     <row r="94" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C94" s="26"/>
+      <c r="C94" s="32"/>
       <c r="D94" s="20"/>
       <c r="E94" s="21" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="95" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C95" s="26"/>
+      <c r="C95" s="32"/>
       <c r="D95" s="20"/>
       <c r="E95" s="21"/>
     </row>
     <row r="96" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C96" s="26"/>
+      <c r="C96" s="32"/>
       <c r="D96" s="20"/>
       <c r="E96" s="21"/>
     </row>
     <row r="97" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C97" s="26" t="s">
+      <c r="C97" s="32" t="s">
         <v>111</v>
       </c>
       <c r="D97" s="20"/>
@@ -2426,52 +2442,52 @@
       </c>
     </row>
     <row r="98" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C98" s="26"/>
+      <c r="C98" s="32"/>
       <c r="D98" s="20"/>
       <c r="E98" s="21" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="99" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C99" s="26"/>
+      <c r="C99" s="32"/>
       <c r="D99" s="20"/>
       <c r="E99" s="21"/>
     </row>
     <row r="100" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C100" s="26"/>
+      <c r="C100" s="32"/>
       <c r="D100" s="20"/>
       <c r="E100" s="21"/>
     </row>
     <row r="101" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C101" s="47" t="s">
+      <c r="C101" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="D101" s="48"/>
-      <c r="E101" s="50" t="s">
+      <c r="D101" s="46"/>
+      <c r="E101" s="48" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="102" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C102" s="47"/>
-      <c r="D102" s="49"/>
-      <c r="E102" s="51"/>
+      <c r="C102" s="45"/>
+      <c r="D102" s="47"/>
+      <c r="E102" s="49"/>
     </row>
     <row r="103" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C103" s="47"/>
+      <c r="C103" s="45"/>
       <c r="D103" s="20"/>
       <c r="E103" s="21" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="104" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C104" s="47"/>
+      <c r="C104" s="45"/>
       <c r="D104" s="20"/>
       <c r="E104" s="21" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="105" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C105" s="55" t="s">
+      <c r="C105" s="38" t="s">
         <v>124</v>
       </c>
       <c r="D105" s="20"/>
@@ -2480,58 +2496,58 @@
       </c>
     </row>
     <row r="106" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C106" s="56"/>
+      <c r="C106" s="39"/>
       <c r="D106" s="20"/>
       <c r="E106" s="22"/>
       <c r="J106" s="16"/>
     </row>
     <row r="107" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C107" s="57"/>
+      <c r="C107" s="40"/>
       <c r="D107" s="20"/>
       <c r="E107" s="21"/>
     </row>
     <row r="108" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C108" s="55" t="s">
+      <c r="C108" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="D108" s="58" t="s">
+      <c r="D108" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="E108" s="59"/>
+      <c r="E108" s="42"/>
     </row>
     <row r="109" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C109" s="56"/>
-      <c r="D109" s="58"/>
-      <c r="E109" s="59"/>
+      <c r="C109" s="39"/>
+      <c r="D109" s="41"/>
+      <c r="E109" s="42"/>
     </row>
     <row r="110" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C110" s="56"/>
+      <c r="C110" s="39"/>
       <c r="D110" s="20"/>
       <c r="E110" s="21" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="111" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C111" s="56"/>
-      <c r="D111" s="60"/>
-      <c r="E111" s="52" t="s">
+      <c r="C111" s="39"/>
+      <c r="D111" s="43"/>
+      <c r="E111" s="33" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="112" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C112" s="56"/>
-      <c r="D112" s="61"/>
-      <c r="E112" s="52"/>
+      <c r="C112" s="39"/>
+      <c r="D112" s="44"/>
+      <c r="E112" s="33"/>
     </row>
     <row r="113" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C113" s="56"/>
+      <c r="C113" s="39"/>
       <c r="D113" s="10" t="s">
         <v>129</v>
       </c>
       <c r="E113" s="10"/>
     </row>
     <row r="114" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C114" s="57"/>
+      <c r="C114" s="40"/>
       <c r="D114" s="10"/>
       <c r="E114" s="10" t="s">
         <v>130</v>
@@ -2542,14 +2558,14 @@
         <v>132</v>
       </c>
       <c r="D115" s="13"/>
-      <c r="E115" s="52" t="s">
+      <c r="E115" s="33" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="116" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C116" s="35"/>
       <c r="D116" s="13"/>
-      <c r="E116" s="52"/>
+      <c r="E116" s="33"/>
     </row>
     <row r="117" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="35"/>
@@ -2559,7 +2575,7 @@
       </c>
     </row>
     <row r="118" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C118" s="53" t="s">
+      <c r="C118" s="36" t="s">
         <v>136</v>
       </c>
       <c r="D118" s="13"/>
@@ -2568,40 +2584,100 @@
       </c>
     </row>
     <row r="119" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C119" s="54"/>
+      <c r="C119" s="37"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
     <row r="120" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C120" s="54"/>
+      <c r="C120" s="37"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
     <row r="121" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C121" s="54"/>
+      <c r="C121" s="37"/>
       <c r="D121" s="10"/>
       <c r="E121" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="119">
-    <mergeCell ref="H88:H92"/>
-    <mergeCell ref="H61:H74"/>
-    <mergeCell ref="I75:I77"/>
-    <mergeCell ref="J79:J80"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="H75:H80"/>
-    <mergeCell ref="J81:J82"/>
-    <mergeCell ref="J83:J84"/>
-    <mergeCell ref="H81:H87"/>
-    <mergeCell ref="C115:C117"/>
-    <mergeCell ref="E115:E116"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C105:C107"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="C108:C114"/>
+  <mergeCells count="121">
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="C93:C96"/>
+    <mergeCell ref="E80:E82"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="J62:J65"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="I67:I69"/>
+    <mergeCell ref="J67:J69"/>
+    <mergeCell ref="I70:I71"/>
+    <mergeCell ref="J73:J74"/>
+    <mergeCell ref="J88:J89"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="D42:D46"/>
+    <mergeCell ref="E42:E46"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="H46:H50"/>
+    <mergeCell ref="M46:M49"/>
+    <mergeCell ref="M50:M52"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="M53:M55"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="M56:M57"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="H23:H27"/>
+    <mergeCell ref="M25:M29"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="H28:H32"/>
+    <mergeCell ref="I28:I32"/>
+    <mergeCell ref="J28:J32"/>
+    <mergeCell ref="M30:M34"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M20:M24"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
     <mergeCell ref="C97:C100"/>
     <mergeCell ref="C101:C104"/>
     <mergeCell ref="D89:D90"/>
@@ -2626,83 +2702,25 @@
     <mergeCell ref="O10:O12"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M20:M24"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="M25:M29"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="H28:H32"/>
-    <mergeCell ref="I28:I32"/>
-    <mergeCell ref="J28:J32"/>
-    <mergeCell ref="M30:M34"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="O30:O32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="C37:C41"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="D42:D46"/>
-    <mergeCell ref="E42:E46"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="H46:H50"/>
-    <mergeCell ref="M46:M49"/>
-    <mergeCell ref="M50:M52"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="M53:M55"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="M56:M57"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="C93:C96"/>
-    <mergeCell ref="E80:E82"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="J62:J65"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="I67:I69"/>
-    <mergeCell ref="J67:J69"/>
-    <mergeCell ref="I70:I71"/>
-    <mergeCell ref="J73:J74"/>
+    <mergeCell ref="C115:C117"/>
+    <mergeCell ref="E115:E116"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C105:C107"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="C108:C114"/>
+    <mergeCell ref="H61:H74"/>
+    <mergeCell ref="I75:I77"/>
+    <mergeCell ref="J79:J80"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="H75:H80"/>
+    <mergeCell ref="J81:J82"/>
+    <mergeCell ref="J83:J84"/>
+    <mergeCell ref="H81:H87"/>
+    <mergeCell ref="H88:H89"/>
+    <mergeCell ref="I88:I89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Adicionar favoritos + pedir ajuda to sequence diagram
</commit_message>
<xml_diff>
--- a/projeto/Especificação de Use Cases.XLSX
+++ b/projeto/Especificação de Use Cases.XLSX
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guilhermeviveiros/Desktop/Documentos/2-semestre/LI4/projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CésarAugustodaCostaB\Documents\Projects\LI4\projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7C4B4E-441B-5942-B232-D9E740652B18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6D7759-6EB1-4366-8ADE-7006D2FB2225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="162">
   <si>
     <t>Use Case:</t>
   </si>
@@ -417,36 +417,12 @@
     <t>Ementa semanal foi alterada</t>
   </si>
   <si>
-    <t>2. Escolhe uma receita</t>
-  </si>
-  <si>
-    <t>3. Escolhe uma refeição e dia da semana</t>
-  </si>
-  <si>
-    <t>4. Escolhe adicionar uma receita à ementa</t>
-  </si>
-  <si>
-    <t>5. Verifica escolhas</t>
-  </si>
-  <si>
-    <t>6. Adiciona receita à ementa</t>
-  </si>
-  <si>
     <t>Encontrou pelo menos uma receita</t>
   </si>
   <si>
     <t>Comportamento Alternativo 1 [Escolhe remover uma receita] (passo 4)</t>
   </si>
   <si>
-    <t>4.1 Escolhe remover uma receita da ementa</t>
-  </si>
-  <si>
-    <t>4.2 Verifica escolhas</t>
-  </si>
-  <si>
-    <t>4.2 Remove receita da ementa</t>
-  </si>
-  <si>
     <t>Comportamento Alternativo 2 [Já existe receita para aquela refeição e dia] (passo 5)</t>
   </si>
   <si>
@@ -468,9 +444,6 @@
     <t>5.5 Volta ao passo 6</t>
   </si>
   <si>
-    <t>5.3.1 Termina editar ementa semanal</t>
-  </si>
-  <si>
     <t>2.2. &lt;include&gt; Apagar Conta</t>
   </si>
   <si>
@@ -487,6 +460,57 @@
   </si>
   <si>
     <t>2.1Informa que o email ou pass são invalidos</t>
+  </si>
+  <si>
+    <t>1. Mostra todas as receitas na ementa nos dias e refeições já escolhidas</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Extends&gt;&gt; adicionar receita à ementa</t>
+  </si>
+  <si>
+    <t>4.1 &lt;&lt;Extends&gt;&gt; remover receita da ementa</t>
+  </si>
+  <si>
+    <t>Adcionar receita à ementa</t>
+  </si>
+  <si>
+    <t>receita adicionada</t>
+  </si>
+  <si>
+    <t>1. Escolhe dia e refeição</t>
+  </si>
+  <si>
+    <t>2. Valida escolha</t>
+  </si>
+  <si>
+    <t>3. Adiciona receita à ementa</t>
+  </si>
+  <si>
+    <t>5.3.1 Informa que não foi adiciona a receita</t>
+  </si>
+  <si>
+    <t>Remover receita da ementa</t>
+  </si>
+  <si>
+    <t>3. Remove receita da ementa</t>
+  </si>
+  <si>
+    <t>Pedir ajudar</t>
+  </si>
+  <si>
+    <t>1. Solicita ajuda num certo conceito</t>
+  </si>
+  <si>
+    <t>2. Procura conceito</t>
+  </si>
+  <si>
+    <t>3. Mostra uma descrição, e possivelmente uma imagem e/ou video sobre o conceito</t>
+  </si>
+  <si>
+    <t>Exceção 1 [não existe conceito] (passo 4)</t>
+  </si>
+  <si>
+    <t>2.1 Informa que é possível encontrar esse conceito</t>
   </si>
 </sst>
 </file>
@@ -510,7 +534,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -569,6 +593,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFBDD7EE"/>
       </patternFill>
     </fill>
   </fills>
@@ -645,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -705,146 +735,158 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1230,99 +1272,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:O118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" zoomScale="101" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O62" sqref="O62"/>
+    <sheetView tabSelected="1" topLeftCell="B63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="1" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" customWidth="1"/>
-    <col min="9" max="9" width="21.1640625" customWidth="1"/>
-    <col min="10" max="10" width="23.1640625" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" customWidth="1"/>
-    <col min="12" max="12" width="8.5" customWidth="1"/>
-    <col min="13" max="13" width="20.83203125" customWidth="1"/>
-    <col min="14" max="14" width="23.5" customWidth="1"/>
-    <col min="15" max="15" width="22.1640625" customWidth="1"/>
-    <col min="16" max="1025" width="8.5" customWidth="1"/>
+    <col min="6" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" customWidth="1"/>
+    <col min="16" max="1025" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="49"/>
       <c r="H4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="31"/>
+      <c r="J4" s="49"/>
       <c r="M4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="31" t="s">
+      <c r="N4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="31"/>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="O4" s="49"/>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="49"/>
       <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="31"/>
+      <c r="J5" s="49"/>
       <c r="M5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="31"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="O5" s="49"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="31"/>
+      <c r="D6" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="49"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="31"/>
+      <c r="J6" s="49"/>
       <c r="M6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="31"/>
-    </row>
-    <row r="7" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="44" t="s">
+      <c r="O6" s="49"/>
+    </row>
+    <row r="7" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="48" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1331,7 +1373,7 @@
       <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="48" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1340,7 +1382,7 @@
       <c r="J7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="44" t="s">
+      <c r="M7" s="48" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="2" t="s">
@@ -1350,102 +1392,102 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="3:15" ht="32" x14ac:dyDescent="0.2">
-      <c r="C8" s="44"/>
+    <row r="8" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="48"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="H8" s="44"/>
+      <c r="H8" s="48"/>
       <c r="I8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="M8" s="44"/>
+      <c r="M8" s="48"/>
       <c r="N8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="44"/>
+    <row r="9" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="48"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="44"/>
+      <c r="H9" s="48"/>
       <c r="I9" s="50"/>
-      <c r="J9" s="47" t="s">
+      <c r="J9" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="44"/>
+      <c r="M9" s="48"/>
       <c r="N9" s="3"/>
       <c r="O9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="44"/>
+    <row r="10" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="48"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="44"/>
+      <c r="H10" s="48"/>
       <c r="I10" s="50"/>
-      <c r="J10" s="47"/>
-      <c r="M10" s="44"/>
+      <c r="J10" s="51"/>
+      <c r="M10" s="48"/>
       <c r="N10" s="50"/>
-      <c r="O10" s="49" t="s">
+      <c r="O10" s="52" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="3:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="C11" s="44"/>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="48"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="44"/>
+      <c r="H11" s="48"/>
       <c r="I11" s="50"/>
-      <c r="J11" s="47"/>
-      <c r="M11" s="44"/>
+      <c r="J11" s="51"/>
+      <c r="M11" s="48"/>
       <c r="N11" s="50"/>
-      <c r="O11" s="49"/>
-    </row>
-    <row r="12" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="30" t="s">
+      <c r="O11" s="52"/>
+    </row>
+    <row r="12" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="42" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="47" t="s">
+      <c r="H12" s="48"/>
+      <c r="I12" s="51" t="s">
         <v>24</v>
       </c>
       <c r="J12" s="50"/>
-      <c r="M12" s="44"/>
+      <c r="M12" s="48"/>
       <c r="N12" s="50"/>
-      <c r="O12" s="49"/>
-    </row>
-    <row r="13" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="30"/>
+      <c r="O12" s="52"/>
+    </row>
+    <row r="13" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="42"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="44"/>
-      <c r="I13" s="47"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="51"/>
       <c r="J13" s="50"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="49" t="s">
+      <c r="M13" s="48"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="52" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="3:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="C14" s="30"/>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="42"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
         <v>27</v>
@@ -1453,11 +1495,11 @@
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="49"/>
-    </row>
-    <row r="15" spans="3:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="M14" s="48"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="52"/>
+    </row>
+    <row r="15" spans="3:15" ht="45" x14ac:dyDescent="0.25">
       <c r="C15" s="7" t="s">
         <v>28</v>
       </c>
@@ -1468,101 +1510,101 @@
       <c r="H15" s="8"/>
       <c r="I15" s="6"/>
       <c r="J15" s="9"/>
-      <c r="M15" s="44"/>
+      <c r="M15" s="48"/>
       <c r="N15" s="4" t="s">
         <v>30</v>
       </c>
       <c r="O15" s="10"/>
     </row>
-    <row r="16" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M16" s="44"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="49" t="s">
+    <row r="16" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M16" s="48"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="52" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="M17" s="44"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="49"/>
-    </row>
-    <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M18" s="44"/>
-      <c r="N18" s="49" t="s">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M17" s="48"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="52"/>
+    </row>
+    <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="48"/>
+      <c r="N18" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="O18" s="51"/>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="M19" s="44"/>
-      <c r="N19" s="49"/>
-      <c r="O19" s="51"/>
-    </row>
-    <row r="20" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O18" s="53"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M19" s="48"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="53"/>
+    </row>
+    <row r="20" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="31"/>
+      <c r="E20" s="49"/>
       <c r="H20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I20" s="31" t="s">
+      <c r="I20" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="31"/>
-      <c r="M20" s="30" t="s">
+      <c r="J20" s="49"/>
+      <c r="M20" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="N20" s="47" t="s">
+      <c r="N20" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="O20" s="48"/>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="O20" s="54"/>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="31"/>
+      <c r="E21" s="49"/>
       <c r="H21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="31"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="48"/>
-    </row>
-    <row r="22" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J21" s="49"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="54"/>
+    </row>
+    <row r="22" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="31"/>
+      <c r="E22" s="49"/>
       <c r="H22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="31" t="s">
+      <c r="I22" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="J22" s="31"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="49" t="s">
+      <c r="J22" s="49"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="52" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="40" t="s">
+    <row r="23" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="55" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1571,7 +1613,7 @@
       <c r="E23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="40" t="s">
+      <c r="H23" s="55" t="s">
         <v>10</v>
       </c>
       <c r="I23" s="2" t="s">
@@ -1580,103 +1622,103 @@
       <c r="J23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="30"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="49"/>
-    </row>
-    <row r="24" spans="3:15" ht="32" x14ac:dyDescent="0.2">
-      <c r="C24" s="40"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="52"/>
+    </row>
+    <row r="24" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C24" s="55"/>
       <c r="D24" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="H24" s="40"/>
+      <c r="H24" s="55"/>
       <c r="I24" s="3" t="s">
         <v>41</v>
       </c>
       <c r="J24" s="3"/>
-      <c r="M24" s="30"/>
+      <c r="M24" s="42"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="40"/>
+    <row r="25" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="55"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="40"/>
+      <c r="H25" s="55"/>
       <c r="I25" s="10"/>
       <c r="J25" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="M25" s="30" t="s">
+      <c r="M25" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="47" t="s">
+      <c r="N25" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="O25" s="48"/>
-    </row>
-    <row r="26" spans="3:15" ht="32" x14ac:dyDescent="0.2">
-      <c r="C26" s="40"/>
+      <c r="O25" s="54"/>
+    </row>
+    <row r="26" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26" s="55"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H26" s="40"/>
+      <c r="H26" s="55"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="M26" s="30"/>
-      <c r="N26" s="47"/>
-      <c r="O26" s="48"/>
-    </row>
-    <row r="27" spans="3:15" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M26" s="42"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="54"/>
+    </row>
+    <row r="27" spans="3:15" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="8"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="H27" s="40"/>
+      <c r="H27" s="55"/>
       <c r="I27" s="19"/>
       <c r="J27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M27" s="30"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="49" t="s">
+      <c r="M27" s="42"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H28" s="41" t="s">
+    <row r="28" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="I28" s="42"/>
-      <c r="J28" s="43" t="s">
+      <c r="I28" s="57"/>
+      <c r="J28" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="M28" s="30"/>
-      <c r="N28" s="48"/>
-      <c r="O28" s="49"/>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="H29" s="41"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="43"/>
-      <c r="M29" s="30"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="54"/>
+      <c r="O28" s="52"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H29" s="56"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="58"/>
+      <c r="M29" s="42"/>
       <c r="N29" s="11"/>
       <c r="O29" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H30" s="41"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="43"/>
-      <c r="M30" s="30" t="s">
+    <row r="30" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="56"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="58"/>
+      <c r="M30" s="42" t="s">
         <v>53</v>
       </c>
       <c r="N30" s="50"/>
@@ -1684,61 +1726,61 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="H31" s="41"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="43"/>
-      <c r="M31" s="30"/>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H31" s="56"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="58"/>
+      <c r="M31" s="42"/>
       <c r="N31" s="50"/>
       <c r="O31" s="50"/>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="H32" s="41"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="43"/>
-      <c r="M32" s="30"/>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H32" s="56"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="58"/>
+      <c r="M32" s="42"/>
       <c r="N32" s="50"/>
       <c r="O32" s="50"/>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="M33" s="30"/>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M33" s="42"/>
       <c r="N33" s="10"/>
       <c r="O33" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="31" t="s">
+      <c r="D34" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="M34" s="30"/>
+      <c r="E34" s="49"/>
+      <c r="M34" s="42"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="31"/>
-    </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="E35" s="49"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="31"/>
-    </row>
-    <row r="37" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="40" t="s">
+      <c r="E36" s="49"/>
+    </row>
+    <row r="37" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="55" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -1748,105 +1790,105 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="3:15" ht="32" x14ac:dyDescent="0.2">
-      <c r="C38" s="40"/>
+    <row r="38" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C38" s="55"/>
       <c r="D38" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="3:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="C39" s="40"/>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C39" s="55"/>
       <c r="D39" s="10"/>
       <c r="E39" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="3:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="C40" s="40"/>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C40" s="55"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="3:15" ht="32" x14ac:dyDescent="0.2">
-      <c r="C41" s="40"/>
+    <row r="41" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C41" s="55"/>
       <c r="D41" s="17"/>
       <c r="E41" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C42" s="41" t="s">
+    <row r="42" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="42"/>
-      <c r="E42" s="43" t="s">
+      <c r="D42" s="57"/>
+      <c r="E42" s="58" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C43" s="41"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="43"/>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="56"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="58"/>
       <c r="H43" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I43" s="31" t="s">
+      <c r="I43" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="J43" s="31"/>
+      <c r="J43" s="49"/>
       <c r="M43" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N43" s="31" t="s">
+      <c r="N43" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="O43" s="31"/>
-    </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C44" s="41"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="43"/>
+      <c r="O43" s="49"/>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C44" s="56"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="58"/>
       <c r="H44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I44" s="31" t="s">
+      <c r="I44" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="J44" s="31"/>
+      <c r="J44" s="49"/>
       <c r="M44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N44" s="31" t="s">
+      <c r="N44" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O44" s="31"/>
-    </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="43"/>
+      <c r="O44" s="49"/>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C45" s="56"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="58"/>
       <c r="H45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I45" s="31" t="s">
+      <c r="I45" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="J45" s="31"/>
+      <c r="J45" s="49"/>
       <c r="M45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N45" s="31" t="s">
+      <c r="N45" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="O45" s="31"/>
-    </row>
-    <row r="46" spans="3:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="41"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="43"/>
-      <c r="H46" s="44" t="s">
+      <c r="O45" s="49"/>
+    </row>
+    <row r="46" spans="3:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="56"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="58"/>
+      <c r="H46" s="48" t="s">
         <v>10</v>
       </c>
       <c r="I46" s="2" t="s">
@@ -1855,7 +1897,7 @@
       <c r="J46" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M46" s="45" t="s">
+      <c r="M46" s="59" t="s">
         <v>10</v>
       </c>
       <c r="N46" s="2" t="s">
@@ -1865,49 +1907,49 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="3:15" ht="48" x14ac:dyDescent="0.2">
-      <c r="H47" s="44"/>
+    <row r="47" spans="3:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="H47" s="48"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="M47" s="45"/>
+      <c r="M47" s="59"/>
       <c r="N47" s="13" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="O47" s="13"/>
     </row>
-    <row r="48" spans="3:15" ht="32" x14ac:dyDescent="0.2">
-      <c r="H48" s="44"/>
+    <row r="48" spans="3:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="H48" s="48"/>
       <c r="I48" s="13" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="J48" s="13"/>
-      <c r="M48" s="45"/>
+      <c r="M48" s="59"/>
       <c r="N48" s="13"/>
       <c r="O48" s="13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="49" spans="3:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="H49" s="44"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H49" s="48"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="M49" s="45"/>
+      <c r="M49" s="59"/>
       <c r="N49" s="13"/>
       <c r="O49" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="3:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H50" s="44"/>
+    <row r="50" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="48"/>
       <c r="I50" s="13"/>
       <c r="J50" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="M50" s="30" t="s">
+      <c r="M50" s="42" t="s">
         <v>73</v>
       </c>
       <c r="N50" s="13"/>
@@ -1915,56 +1957,56 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="3:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D51" s="31" t="s">
+      <c r="D51" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="E51" s="31"/>
-      <c r="H51" s="30" t="s">
+      <c r="E51" s="49"/>
+      <c r="H51" s="42" t="s">
         <v>76</v>
       </c>
       <c r="I51" s="13"/>
       <c r="J51" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M51" s="30"/>
+      <c r="M51" s="42"/>
       <c r="N51" s="13"/>
       <c r="O51" s="13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C52" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="31" t="s">
+      <c r="D52" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="31"/>
-      <c r="H52" s="30"/>
+      <c r="E52" s="49"/>
+      <c r="H52" s="42"/>
       <c r="I52" s="13"/>
       <c r="J52" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="M52" s="30"/>
+      <c r="M52" s="42"/>
       <c r="N52" s="13"/>
       <c r="O52" s="13"/>
     </row>
-    <row r="53" spans="3:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="31" t="s">
+      <c r="D53" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="E53" s="31"/>
-      <c r="H53" s="30"/>
+      <c r="E53" s="49"/>
+      <c r="H53" s="42"/>
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
-      <c r="M53" s="38" t="s">
+      <c r="M53" s="32" t="s">
         <v>81</v>
       </c>
       <c r="N53" s="13"/>
@@ -1972,8 +2014,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C54" s="45" t="s">
+    <row r="54" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="59" t="s">
         <v>10</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -1982,46 +2024,46 @@
       <c r="E54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M54" s="38"/>
+      <c r="M54" s="32"/>
       <c r="N54" s="13"/>
       <c r="O54" s="13"/>
     </row>
-    <row r="55" spans="3:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="C55" s="45"/>
+    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C55" s="59"/>
       <c r="D55" s="13" t="s">
         <v>83</v>
       </c>
       <c r="E55" s="13"/>
-      <c r="M55" s="38"/>
+      <c r="M55" s="32"/>
       <c r="N55" s="13"/>
       <c r="O55" s="13"/>
     </row>
-    <row r="56" spans="3:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C56" s="45"/>
+    <row r="56" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="59"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="M56" s="46" t="s">
+      <c r="M56" s="60" t="s">
         <v>85</v>
       </c>
       <c r="N56" s="13"/>
       <c r="O56" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="3:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="C57" s="45"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C57" s="59"/>
       <c r="D57" s="13" t="s">
         <v>86</v>
       </c>
       <c r="E57" s="10"/>
-      <c r="M57" s="46"/>
+      <c r="M57" s="60"/>
       <c r="N57" s="13"/>
       <c r="O57" s="13"/>
     </row>
-    <row r="58" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C58" s="37" t="s">
+    <row r="58" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="64" t="s">
         <v>87</v>
       </c>
       <c r="D58" s="13" t="s">
@@ -2031,44 +2073,44 @@
       <c r="H58" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I58" s="31" t="s">
+      <c r="I58" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="J58" s="31"/>
-    </row>
-    <row r="59" spans="3:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="C59" s="37"/>
+      <c r="J58" s="49"/>
+    </row>
+    <row r="59" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C59" s="64"/>
       <c r="D59" s="13"/>
       <c r="E59" s="13" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="H59" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I59" s="31" t="s">
+      <c r="I59" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="J59" s="31"/>
-    </row>
-    <row r="60" spans="3:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="C60" s="37"/>
+      <c r="J59" s="49"/>
+    </row>
+    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C60" s="64"/>
       <c r="D60" s="13"/>
       <c r="E60" s="13" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H60" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I60" s="31" t="s">
+      <c r="I60" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="J60" s="31"/>
-    </row>
-    <row r="61" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C61" s="37"/>
+      <c r="J60" s="49"/>
+    </row>
+    <row r="61" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="64"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
-      <c r="H61" s="44" t="s">
+      <c r="H61" s="48" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="2" t="s">
@@ -2077,71 +2119,117 @@
       <c r="J61" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="H62" s="44"/>
+      <c r="M61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N61" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="O61" s="49"/>
+    </row>
+    <row r="62" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H62" s="48"/>
       <c r="I62" s="13"/>
-      <c r="J62" s="25"/>
-    </row>
-    <row r="63" spans="3:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="H63" s="44"/>
-      <c r="I63" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="J63" s="13"/>
-    </row>
-    <row r="64" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H64" s="44"/>
-      <c r="I64" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="J64" s="32"/>
-    </row>
-    <row r="65" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="H65" s="44"/>
-      <c r="I65" s="35"/>
-      <c r="J65" s="39"/>
-    </row>
-    <row r="66" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="J62" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="M62" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N62" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="O62" s="49"/>
+    </row>
+    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H63" s="48"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="31"/>
+      <c r="M63" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N63" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="O63" s="49"/>
+    </row>
+    <row r="64" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H64" s="48"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="31"/>
+      <c r="M64" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O64" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H65" s="48"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="65"/>
+      <c r="M65" s="71"/>
+      <c r="N65" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="O65" s="13"/>
+    </row>
+    <row r="66" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C66" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D66" s="31" t="s">
+      <c r="D66" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="E66" s="31"/>
-      <c r="H66" s="44"/>
-      <c r="I66" s="36"/>
-      <c r="J66" s="33"/>
-    </row>
-    <row r="67" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="E66" s="49"/>
+      <c r="H66" s="48"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="M66" s="71"/>
+      <c r="N66" s="13"/>
+      <c r="O66" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="31" t="s">
+      <c r="D67" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E67" s="31"/>
-      <c r="H67" s="44"/>
-      <c r="I67" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="J67" s="13"/>
-    </row>
-    <row r="68" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="E67" s="49"/>
+      <c r="H67" s="48"/>
+      <c r="I67" s="30"/>
+      <c r="J67" s="66" t="s">
+        <v>146</v>
+      </c>
+      <c r="M67" s="71"/>
+      <c r="N67" s="13"/>
+      <c r="O67" s="30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C68" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="31" t="s">
+      <c r="D68" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="E68" s="31"/>
-      <c r="H68" s="44"/>
-      <c r="I68" s="33"/>
-      <c r="J68" s="13"/>
-    </row>
-    <row r="69" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C69" s="44" t="s">
+      <c r="E68" s="49"/>
+      <c r="H68" s="48"/>
+      <c r="I68" s="31"/>
+      <c r="J68" s="67"/>
+      <c r="M68" s="71"/>
+      <c r="N68" s="13"/>
+      <c r="O68" s="65"/>
+    </row>
+    <row r="69" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C69" s="48" t="s">
         <v>10</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -2150,249 +2238,351 @@
       <c r="E69" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="44"/>
-      <c r="I69" s="10"/>
-      <c r="J69" s="10" t="s">
+      <c r="H69" s="59"/>
+      <c r="I69" s="31"/>
+      <c r="J69" s="67"/>
+      <c r="M69" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="N69" s="10"/>
+      <c r="O69" s="61" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C70" s="44"/>
-      <c r="D70" s="34"/>
-      <c r="E70" s="34" t="s">
+    <row r="70" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="48"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="H70" s="44"/>
-      <c r="I70" s="10"/>
-      <c r="J70" s="27" t="s">
+      <c r="H70" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="I70" s="29"/>
+      <c r="J70" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="M70" s="72"/>
+      <c r="N70" s="10"/>
+      <c r="O70" s="61"/>
+    </row>
+    <row r="71" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C71" s="48"/>
+      <c r="D71" s="65"/>
+      <c r="E71" s="65"/>
+      <c r="H71" s="42"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="39"/>
+      <c r="M71" s="72"/>
+      <c r="N71" s="10"/>
+      <c r="O71" s="33" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C71" s="44"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
-      <c r="H71" s="44"/>
-      <c r="I71" s="10"/>
-      <c r="J71" s="27"/>
-    </row>
-    <row r="72" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C72" s="44"/>
+    <row r="72" spans="3:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="48"/>
       <c r="D72" s="15" t="s">
         <v>92</v>
       </c>
       <c r="E72" s="11"/>
-      <c r="H72" s="30" t="s">
+      <c r="H72" s="42"/>
+      <c r="I72" s="29"/>
+      <c r="J72" s="39"/>
+      <c r="M72" s="72"/>
+      <c r="N72" s="10"/>
+      <c r="O72" s="33"/>
+    </row>
+    <row r="73" spans="3:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="48"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="H73" s="42"/>
+      <c r="I73" s="75"/>
+      <c r="J73" s="21"/>
+      <c r="M73" s="72"/>
+      <c r="N73" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="O73" s="10"/>
+    </row>
+    <row r="74" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C74" s="48"/>
+      <c r="D74" s="65"/>
+      <c r="E74" s="65"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="27"/>
+      <c r="J74" s="25"/>
+      <c r="M74" s="72"/>
+      <c r="N74" s="10"/>
+      <c r="O74" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="I72" s="67" t="s">
-        <v>137</v>
-      </c>
-      <c r="J72" s="21"/>
-    </row>
-    <row r="73" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C73" s="44"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="H73" s="30"/>
-      <c r="I73" s="68"/>
-      <c r="J73" s="21"/>
-    </row>
-    <row r="74" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C74" s="44"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="H74" s="30"/>
-      <c r="I74" s="69"/>
-      <c r="J74" s="21"/>
-    </row>
-    <row r="75" spans="3:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="C75" s="44"/>
+    </row>
+    <row r="75" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C75" s="48"/>
       <c r="D75" s="15" t="s">
         <v>94</v>
       </c>
       <c r="E75" s="15"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="23"/>
-      <c r="J75" s="21" t="s">
+      <c r="H75" s="26"/>
+      <c r="I75" s="27"/>
+      <c r="J75" s="25"/>
+      <c r="M75" s="72"/>
+      <c r="N75" s="10"/>
+      <c r="O75" s="10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="76" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C76" s="44"/>
+    <row r="76" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="48"/>
       <c r="D76" s="15"/>
       <c r="E76" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H76" s="30"/>
-      <c r="I76" s="32"/>
-      <c r="J76" s="27" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="77" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C77" s="44"/>
+      <c r="H76" s="26"/>
+      <c r="I76" s="28"/>
+      <c r="J76" s="27"/>
+      <c r="M76" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="N76" s="40"/>
+      <c r="O76" s="61" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C77" s="48"/>
       <c r="D77" s="15"/>
-      <c r="E77" s="27" t="s">
+      <c r="E77" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="H77" s="30"/>
-      <c r="I77" s="33"/>
-      <c r="J77" s="27"/>
-      <c r="M77" s="16"/>
-    </row>
-    <row r="78" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C78" s="44"/>
+      <c r="H77" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I77" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="J77" s="49"/>
+      <c r="M77" s="73"/>
+      <c r="N77" s="41"/>
+      <c r="O77" s="61"/>
+    </row>
+    <row r="78" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="48"/>
       <c r="D78" s="15"/>
-      <c r="E78" s="27"/>
-      <c r="H78" s="70" t="s">
-        <v>140</v>
-      </c>
-      <c r="I78" s="10"/>
-      <c r="J78" s="27" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="79" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C79" s="44"/>
+      <c r="E78" s="61"/>
+      <c r="H78" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I78" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="J78" s="49"/>
+    </row>
+    <row r="79" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="48"/>
       <c r="D79" s="15"/>
-      <c r="E79" s="27"/>
-      <c r="H79" s="70"/>
-      <c r="I79" s="10"/>
-      <c r="J79" s="27"/>
-    </row>
-    <row r="80" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C80" s="44"/>
-      <c r="D80" s="27" t="s">
+      <c r="E79" s="61"/>
+      <c r="H79" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I79" s="49"/>
+      <c r="J79" s="49"/>
+    </row>
+    <row r="80" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="48"/>
+      <c r="D80" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="E80" s="28"/>
-      <c r="H80" s="70"/>
-      <c r="I80" s="10"/>
-      <c r="J80" s="57" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="81" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C81" s="44"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="29"/>
-      <c r="H81" s="70"/>
-      <c r="I81" s="10"/>
-      <c r="J81" s="57"/>
-    </row>
-    <row r="82" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C82" s="44"/>
+      <c r="E80" s="62"/>
+      <c r="H80" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M80" s="16"/>
+    </row>
+    <row r="81" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C81" s="48"/>
+      <c r="D81" s="61"/>
+      <c r="E81" s="63"/>
+      <c r="H81" s="48"/>
+      <c r="I81" s="66" t="s">
+        <v>157</v>
+      </c>
+      <c r="J81" s="29"/>
+      <c r="M81" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N81" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="O81" s="49"/>
+    </row>
+    <row r="82" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C82" s="48"/>
       <c r="D82" s="11" t="s">
         <v>98</v>
       </c>
       <c r="E82" s="11"/>
-      <c r="H82" s="70"/>
-      <c r="I82" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="J82" s="10"/>
-    </row>
-    <row r="83" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C83" s="44"/>
+      <c r="H82" s="48"/>
+      <c r="I82" s="74"/>
+      <c r="J82" s="29"/>
+      <c r="M82" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N82" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="O82" s="49"/>
+    </row>
+    <row r="83" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C83" s="48"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="H83" s="70"/>
-      <c r="I83" s="10"/>
-      <c r="J83" s="24" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C84" s="44"/>
+      <c r="H83" s="48"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="M83" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N83" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="O83" s="49"/>
+    </row>
+    <row r="84" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="48"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H84" s="70"/>
-      <c r="I84" s="10"/>
-      <c r="J84" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="85" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C85" s="44"/>
+      <c r="H84" s="48"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="M84" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="N84" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O84" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C85" s="48"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="H85" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="I85" s="65"/>
-      <c r="J85" s="27" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="86" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C86" s="44"/>
-      <c r="D86" s="53"/>
-      <c r="E86" s="27" t="s">
+      <c r="H85" s="48"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="29"/>
+      <c r="M85" s="48"/>
+      <c r="N85" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="O85" s="13"/>
+    </row>
+    <row r="86" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C86" s="48"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="H86" s="71"/>
-      <c r="I86" s="66"/>
-      <c r="J86" s="27"/>
-    </row>
-    <row r="87" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C87" s="44"/>
-      <c r="D87" s="54"/>
-      <c r="E87" s="27"/>
-      <c r="H87" s="26"/>
-    </row>
-    <row r="88" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C88" s="44"/>
+      <c r="H86" s="48"/>
+      <c r="I86" s="30"/>
+      <c r="J86" s="29"/>
+      <c r="M86" s="48"/>
+      <c r="N86" s="13"/>
+      <c r="O86" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="87" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="48"/>
+      <c r="D87" s="45"/>
+      <c r="E87" s="61"/>
+      <c r="H87" s="48"/>
+      <c r="I87" s="31"/>
+      <c r="J87" s="29"/>
+      <c r="M87" s="48"/>
+      <c r="N87" s="13"/>
+      <c r="O87" s="61" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="88" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C88" s="48"/>
       <c r="D88" s="11" t="s">
         <v>113</v>
       </c>
       <c r="E88" s="11"/>
-      <c r="H88" s="26"/>
-    </row>
-    <row r="89" spans="3:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C89" s="44"/>
+      <c r="H88" s="48"/>
+      <c r="I88" s="31"/>
+      <c r="J88" s="29"/>
+      <c r="M88" s="48"/>
+      <c r="N88" s="13"/>
+      <c r="O88" s="61"/>
+    </row>
+    <row r="89" spans="3:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="48"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="H89" s="26"/>
-    </row>
-    <row r="90" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C90" s="30" t="s">
+      <c r="H89" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="I89" s="69"/>
+      <c r="J89" s="29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="90" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C90" s="42" t="s">
         <v>110</v>
       </c>
       <c r="D90" s="20"/>
       <c r="E90" s="21" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="91" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C91" s="30"/>
+      <c r="H90" s="68"/>
+      <c r="I90" s="70"/>
+      <c r="J90" s="29"/>
+    </row>
+    <row r="91" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C91" s="42"/>
       <c r="D91" s="20"/>
       <c r="E91" s="21" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C92" s="30"/>
+    <row r="92" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C92" s="42"/>
       <c r="D92" s="20"/>
       <c r="E92" s="21"/>
     </row>
-    <row r="93" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C93" s="30"/>
+    <row r="93" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C93" s="42"/>
       <c r="D93" s="20"/>
       <c r="E93" s="21"/>
     </row>
-    <row r="94" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C94" s="30" t="s">
+    <row r="94" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C94" s="42" t="s">
         <v>102</v>
       </c>
       <c r="D94" s="20"/>
@@ -2400,53 +2590,53 @@
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C95" s="30"/>
+    <row r="95" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C95" s="42"/>
       <c r="D95" s="20"/>
       <c r="E95" s="21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="96" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C96" s="30"/>
+    <row r="96" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C96" s="42"/>
       <c r="D96" s="20"/>
       <c r="E96" s="21"/>
     </row>
-    <row r="97" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C97" s="30"/>
+    <row r="97" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C97" s="42"/>
       <c r="D97" s="20"/>
       <c r="E97" s="21"/>
     </row>
-    <row r="98" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C98" s="52" t="s">
+    <row r="98" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C98" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="D98" s="53"/>
-      <c r="E98" s="55" t="s">
+      <c r="D98" s="44"/>
+      <c r="E98" s="46" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C99" s="52"/>
-      <c r="D99" s="54"/>
-      <c r="E99" s="56"/>
-    </row>
-    <row r="100" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C100" s="52"/>
+    <row r="99" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C99" s="43"/>
+      <c r="D99" s="45"/>
+      <c r="E99" s="47"/>
+    </row>
+    <row r="100" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C100" s="43"/>
       <c r="D100" s="20"/>
       <c r="E100" s="21" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C101" s="52"/>
+    <row r="101" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C101" s="43"/>
       <c r="D101" s="20"/>
       <c r="E101" s="21" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C102" s="60" t="s">
+    <row r="102" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C102" s="36" t="s">
         <v>115</v>
       </c>
       <c r="D102" s="20"/>
@@ -2454,87 +2644,87 @@
         <v>116</v>
       </c>
     </row>
-    <row r="103" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C103" s="61"/>
+    <row r="103" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C103" s="37"/>
       <c r="D103" s="20"/>
       <c r="E103" s="22"/>
       <c r="J103" s="16"/>
     </row>
-    <row r="104" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C104" s="62"/>
+    <row r="104" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C104" s="38"/>
       <c r="D104" s="20"/>
       <c r="E104" s="21"/>
     </row>
-    <row r="105" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C105" s="60" t="s">
+    <row r="105" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C105" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="D105" s="63" t="s">
+      <c r="D105" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="E105" s="64"/>
-    </row>
-    <row r="106" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C106" s="61"/>
-      <c r="D106" s="63"/>
-      <c r="E106" s="64"/>
-    </row>
-    <row r="107" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C107" s="61"/>
+      <c r="E105" s="39"/>
+    </row>
+    <row r="106" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C106" s="37"/>
+      <c r="D106" s="29"/>
+      <c r="E106" s="39"/>
+    </row>
+    <row r="107" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C107" s="37"/>
       <c r="D107" s="20"/>
       <c r="E107" s="21" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="108" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C108" s="61"/>
-      <c r="D108" s="65"/>
-      <c r="E108" s="57" t="s">
+    <row r="108" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C108" s="37"/>
+      <c r="D108" s="40"/>
+      <c r="E108" s="33" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C109" s="61"/>
-      <c r="D109" s="66"/>
-      <c r="E109" s="57"/>
-    </row>
-    <row r="110" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C110" s="61"/>
+    <row r="109" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C109" s="37"/>
+      <c r="D109" s="41"/>
+      <c r="E109" s="33"/>
+    </row>
+    <row r="110" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C110" s="37"/>
       <c r="D110" s="10" t="s">
         <v>120</v>
       </c>
       <c r="E110" s="10"/>
     </row>
-    <row r="111" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C111" s="62"/>
+    <row r="111" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C111" s="38"/>
       <c r="D111" s="10"/>
       <c r="E111" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="112" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C112" s="38" t="s">
+    <row r="112" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C112" s="32" t="s">
         <v>123</v>
       </c>
       <c r="D112" s="13"/>
-      <c r="E112" s="57" t="s">
+      <c r="E112" s="33" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="113" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C113" s="38"/>
+    <row r="113" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C113" s="32"/>
       <c r="D113" s="13"/>
-      <c r="E113" s="57"/>
-    </row>
-    <row r="114" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C114" s="38"/>
+      <c r="E113" s="33"/>
+    </row>
+    <row r="114" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C114" s="32"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="115" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C115" s="58" t="s">
+    <row r="115" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C115" s="34" t="s">
         <v>127</v>
       </c>
       <c r="D115" s="13"/>
@@ -2542,98 +2732,64 @@
         <v>124</v>
       </c>
     </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C116" s="59"/>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C116" s="35"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C117" s="59"/>
+    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C117" s="35"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C118" s="59"/>
+    <row r="118" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C118" s="35"/>
       <c r="D118" s="10"/>
       <c r="E118" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="118">
-    <mergeCell ref="H61:H71"/>
-    <mergeCell ref="I72:I74"/>
-    <mergeCell ref="J76:J77"/>
-    <mergeCell ref="I76:I77"/>
-    <mergeCell ref="H72:H77"/>
-    <mergeCell ref="J78:J79"/>
-    <mergeCell ref="J80:J81"/>
-    <mergeCell ref="H78:H84"/>
-    <mergeCell ref="H85:H86"/>
-    <mergeCell ref="I85:I86"/>
-    <mergeCell ref="C112:C114"/>
-    <mergeCell ref="E112:E113"/>
-    <mergeCell ref="C115:C118"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="C105:C111"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="C69:C89"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="H7:H13"/>
-    <mergeCell ref="M7:M19"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="N10:N12"/>
-    <mergeCell ref="O10:O12"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M20:M24"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="M25:M29"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="H28:H32"/>
-    <mergeCell ref="I28:I32"/>
-    <mergeCell ref="J28:J32"/>
-    <mergeCell ref="M30:M34"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="O30:O32"/>
-    <mergeCell ref="D34:E34"/>
+  <mergeCells count="137">
+    <mergeCell ref="H80:H88"/>
+    <mergeCell ref="I81:I82"/>
+    <mergeCell ref="J81:J82"/>
+    <mergeCell ref="I89:I90"/>
+    <mergeCell ref="J89:J90"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="N63:O63"/>
+    <mergeCell ref="M64:M68"/>
+    <mergeCell ref="O67:O68"/>
+    <mergeCell ref="M69:M75"/>
+    <mergeCell ref="O69:O70"/>
+    <mergeCell ref="O71:O72"/>
+    <mergeCell ref="M76:M77"/>
+    <mergeCell ref="N76:N77"/>
+    <mergeCell ref="O76:O77"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="N82:O82"/>
+    <mergeCell ref="N83:O83"/>
+    <mergeCell ref="M84:M88"/>
+    <mergeCell ref="O87:O88"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="I79:J79"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="H61:H69"/>
+    <mergeCell ref="J62:J65"/>
+    <mergeCell ref="I67:I69"/>
+    <mergeCell ref="J67:J69"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="I70:I72"/>
+    <mergeCell ref="J70:J72"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="C37:C41"/>
@@ -2656,27 +2812,80 @@
     <mergeCell ref="M53:M55"/>
     <mergeCell ref="C54:C57"/>
     <mergeCell ref="M56:M57"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="H23:H27"/>
+    <mergeCell ref="M25:M29"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="H28:H32"/>
+    <mergeCell ref="I28:I32"/>
+    <mergeCell ref="J28:J32"/>
+    <mergeCell ref="M30:M34"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M20:M24"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="H7:H13"/>
+    <mergeCell ref="M7:M19"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="N10:N12"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="J84:J88"/>
+    <mergeCell ref="I86:I88"/>
+    <mergeCell ref="C112:C114"/>
+    <mergeCell ref="E112:E113"/>
+    <mergeCell ref="C115:C118"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="C105:C111"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="C69:C89"/>
     <mergeCell ref="E86:E87"/>
     <mergeCell ref="D80:D81"/>
     <mergeCell ref="E80:E81"/>
     <mergeCell ref="C90:C93"/>
     <mergeCell ref="E77:E79"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="I64:I66"/>
-    <mergeCell ref="J64:J66"/>
-    <mergeCell ref="I67:I68"/>
-    <mergeCell ref="J70:J71"/>
-    <mergeCell ref="J85:J86"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="H89:H90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Minor updates to different diagrams + changed Gauss diagram in project
</commit_message>
<xml_diff>
--- a/projeto/Especificação de Use Cases.XLSX
+++ b/projeto/Especificação de Use Cases.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CésarAugustodaCostaB\Documents\Projects\LI4\projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6D7759-6EB1-4366-8ADE-7006D2FB2225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37F6F77-779A-4D0E-ABD4-73D7A4A03F8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -675,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -747,20 +747,104 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -777,18 +861,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -804,89 +876,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1272,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:O118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
@@ -1298,73 +1295,73 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="49"/>
+      <c r="E4" s="35"/>
       <c r="H4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="49"/>
+      <c r="J4" s="35"/>
       <c r="M4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="49" t="s">
+      <c r="N4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="49"/>
+      <c r="O4" s="35"/>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="49"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="49" t="s">
+      <c r="I5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="49"/>
+      <c r="J5" s="35"/>
       <c r="M5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="49" t="s">
+      <c r="N5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="49"/>
+      <c r="O5" s="35"/>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E6" s="49"/>
+      <c r="E6" s="35"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="49" t="s">
+      <c r="I6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="49"/>
+      <c r="J6" s="35"/>
       <c r="M6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="49" t="s">
+      <c r="N6" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="49"/>
+      <c r="O6" s="35"/>
     </row>
     <row r="7" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="29" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1373,7 +1370,7 @@
       <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="29" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1382,7 +1379,7 @@
       <c r="J7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="48" t="s">
+      <c r="M7" s="29" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="2" t="s">
@@ -1393,101 +1390,101 @@
       </c>
     </row>
     <row r="8" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="48"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="H8" s="48"/>
+      <c r="H8" s="29"/>
       <c r="I8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="M8" s="48"/>
+      <c r="M8" s="29"/>
       <c r="N8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="O8" s="3"/>
     </row>
     <row r="9" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="48"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="48"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="51" t="s">
+      <c r="H9" s="29"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="48"/>
+      <c r="M9" s="29"/>
       <c r="N9" s="3"/>
       <c r="O9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="48"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="48"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="51"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="52" t="s">
+      <c r="H10" s="29"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="57"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="59" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="48"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="48"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="51"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="52"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="57"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="59"/>
     </row>
     <row r="12" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="49" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="51" t="s">
+      <c r="H12" s="29"/>
+      <c r="I12" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="50"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="52"/>
+      <c r="J12" s="60"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="59"/>
     </row>
     <row r="13" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="42"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="48"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="50"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="52" t="s">
+      <c r="H13" s="29"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="60"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="59" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="42"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
         <v>27</v>
@@ -1495,9 +1492,9 @@
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="52"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="59"/>
     </row>
     <row r="15" spans="3:15" ht="45" x14ac:dyDescent="0.25">
       <c r="C15" s="7" t="s">
@@ -1510,101 +1507,101 @@
       <c r="H15" s="8"/>
       <c r="I15" s="6"/>
       <c r="J15" s="9"/>
-      <c r="M15" s="48"/>
+      <c r="M15" s="29"/>
       <c r="N15" s="4" t="s">
         <v>30</v>
       </c>
       <c r="O15" s="10"/>
     </row>
     <row r="16" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M16" s="48"/>
-      <c r="N16" s="53"/>
-      <c r="O16" s="52" t="s">
+      <c r="M16" s="29"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="59" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M17" s="48"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="52"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="61"/>
+      <c r="O17" s="59"/>
     </row>
     <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M18" s="48"/>
-      <c r="N18" s="52" t="s">
+      <c r="M18" s="29"/>
+      <c r="N18" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="O18" s="53"/>
+      <c r="O18" s="61"/>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M19" s="48"/>
-      <c r="N19" s="52"/>
-      <c r="O19" s="53"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="61"/>
     </row>
     <row r="20" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="49"/>
+      <c r="E20" s="35"/>
       <c r="H20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="49"/>
-      <c r="M20" s="42" t="s">
+      <c r="J20" s="35"/>
+      <c r="M20" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="N20" s="51" t="s">
+      <c r="N20" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="O20" s="54"/>
+      <c r="O20" s="58"/>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="49"/>
+      <c r="E21" s="35"/>
       <c r="H21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="49" t="s">
+      <c r="I21" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="49"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="54"/>
+      <c r="J21" s="35"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="58"/>
     </row>
     <row r="22" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="49"/>
+      <c r="E22" s="35"/>
       <c r="H22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="49" t="s">
+      <c r="I22" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="J22" s="49"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="52" t="s">
+      <c r="J22" s="35"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="59" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="55" t="s">
+      <c r="C23" s="51" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1613,7 +1610,7 @@
       <c r="E23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="55" t="s">
+      <c r="H23" s="51" t="s">
         <v>10</v>
       </c>
       <c r="I23" s="2" t="s">
@@ -1622,128 +1619,128 @@
       <c r="J23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="42"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="52"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="59"/>
     </row>
     <row r="24" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C24" s="55"/>
+      <c r="C24" s="51"/>
       <c r="D24" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="H24" s="55"/>
+      <c r="H24" s="51"/>
       <c r="I24" s="3" t="s">
         <v>41</v>
       </c>
       <c r="J24" s="3"/>
-      <c r="M24" s="42"/>
+      <c r="M24" s="49"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="55"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="55"/>
+      <c r="H25" s="51"/>
       <c r="I25" s="10"/>
       <c r="J25" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="M25" s="42" t="s">
+      <c r="M25" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="51" t="s">
+      <c r="N25" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="O25" s="54"/>
+      <c r="O25" s="58"/>
     </row>
     <row r="26" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="55"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H26" s="55"/>
+      <c r="H26" s="51"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="M26" s="42"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="54"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="58"/>
     </row>
     <row r="27" spans="3:15" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="8"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="H27" s="55"/>
+      <c r="H27" s="51"/>
       <c r="I27" s="19"/>
       <c r="J27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M27" s="42"/>
-      <c r="N27" s="54"/>
-      <c r="O27" s="52" t="s">
+      <c r="M27" s="49"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="59" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H28" s="56" t="s">
+      <c r="H28" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="I28" s="57"/>
-      <c r="J28" s="58" t="s">
+      <c r="I28" s="53"/>
+      <c r="J28" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="M28" s="42"/>
-      <c r="N28" s="54"/>
-      <c r="O28" s="52"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="59"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H29" s="56"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="58"/>
-      <c r="M29" s="42"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="54"/>
+      <c r="M29" s="49"/>
       <c r="N29" s="11"/>
       <c r="O29" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H30" s="56"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="58"/>
-      <c r="M30" s="42" t="s">
+      <c r="H30" s="52"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="54"/>
+      <c r="M30" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="N30" s="50"/>
-      <c r="O30" s="50" t="s">
+      <c r="N30" s="60"/>
+      <c r="O30" s="60" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H31" s="56"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="58"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="50"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="54"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="60"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H32" s="56"/>
-      <c r="I32" s="57"/>
-      <c r="J32" s="58"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="50"/>
-      <c r="O32" s="50"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="54"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="60"/>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M33" s="42"/>
+      <c r="M33" s="49"/>
       <c r="N33" s="10"/>
       <c r="O33" s="10" t="s">
         <v>55</v>
@@ -1753,11 +1750,11 @@
       <c r="C34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="49" t="s">
+      <c r="D34" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="49"/>
-      <c r="M34" s="42"/>
+      <c r="E34" s="35"/>
+      <c r="M34" s="49"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
     </row>
@@ -1765,22 +1762,22 @@
       <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="49" t="s">
+      <c r="D35" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="49"/>
+      <c r="E35" s="35"/>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="49" t="s">
+      <c r="D36" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="49"/>
+      <c r="E36" s="35"/>
     </row>
     <row r="37" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="55" t="s">
+      <c r="C37" s="51" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -1791,104 +1788,104 @@
       </c>
     </row>
     <row r="38" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C38" s="55"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C39" s="55"/>
+      <c r="C39" s="51"/>
       <c r="D39" s="10"/>
       <c r="E39" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C40" s="55"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="41" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C41" s="55"/>
+      <c r="C41" s="51"/>
       <c r="D41" s="17"/>
       <c r="E41" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="42" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="56" t="s">
+      <c r="C42" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="57"/>
-      <c r="E42" s="58" t="s">
+      <c r="D42" s="53"/>
+      <c r="E42" s="54" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="56"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="58"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="54"/>
       <c r="H43" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I43" s="49" t="s">
+      <c r="I43" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="J43" s="49"/>
+      <c r="J43" s="35"/>
       <c r="M43" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N43" s="49" t="s">
+      <c r="N43" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="O43" s="49"/>
+      <c r="O43" s="35"/>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="56"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="58"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="54"/>
       <c r="H44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I44" s="49" t="s">
+      <c r="I44" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="J44" s="49"/>
+      <c r="J44" s="35"/>
       <c r="M44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N44" s="49" t="s">
+      <c r="N44" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="O44" s="49"/>
+      <c r="O44" s="35"/>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="56"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="58"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="54"/>
       <c r="H45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I45" s="49" t="s">
+      <c r="I45" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="J45" s="49"/>
+      <c r="J45" s="35"/>
       <c r="M45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N45" s="49" t="s">
+      <c r="N45" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="O45" s="49"/>
+      <c r="O45" s="35"/>
     </row>
     <row r="46" spans="3:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="56"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="58"/>
-      <c r="H46" s="48" t="s">
+      <c r="C46" s="52"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="54"/>
+      <c r="H46" s="29" t="s">
         <v>10</v>
       </c>
       <c r="I46" s="2" t="s">
@@ -1897,7 +1894,7 @@
       <c r="J46" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M46" s="59" t="s">
+      <c r="M46" s="36" t="s">
         <v>10</v>
       </c>
       <c r="N46" s="2" t="s">
@@ -1908,48 +1905,48 @@
       </c>
     </row>
     <row r="47" spans="3:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="H47" s="48"/>
+      <c r="H47" s="29"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="M47" s="59"/>
+      <c r="M47" s="36"/>
       <c r="N47" s="13" t="s">
         <v>142</v>
       </c>
       <c r="O47" s="13"/>
     </row>
     <row r="48" spans="3:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="H48" s="48"/>
+      <c r="H48" s="29"/>
       <c r="I48" s="13" t="s">
         <v>141</v>
       </c>
       <c r="J48" s="13"/>
-      <c r="M48" s="59"/>
+      <c r="M48" s="36"/>
       <c r="N48" s="13"/>
       <c r="O48" s="13" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="49" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H49" s="48"/>
+      <c r="H49" s="29"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="M49" s="59"/>
+      <c r="M49" s="36"/>
       <c r="N49" s="13"/>
       <c r="O49" s="10" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="50" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H50" s="48"/>
+      <c r="H50" s="29"/>
       <c r="I50" s="13"/>
       <c r="J50" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="M50" s="42" t="s">
+      <c r="M50" s="49" t="s">
         <v>73</v>
       </c>
       <c r="N50" s="13"/>
@@ -1961,18 +1958,18 @@
       <c r="C51" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D51" s="49" t="s">
+      <c r="D51" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="E51" s="49"/>
-      <c r="H51" s="42" t="s">
+      <c r="E51" s="35"/>
+      <c r="H51" s="49" t="s">
         <v>76</v>
       </c>
       <c r="I51" s="13"/>
       <c r="J51" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M51" s="42"/>
+      <c r="M51" s="49"/>
       <c r="N51" s="13"/>
       <c r="O51" s="13" t="s">
         <v>78</v>
@@ -1982,16 +1979,16 @@
       <c r="C52" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="49" t="s">
+      <c r="D52" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="49"/>
-      <c r="H52" s="42"/>
+      <c r="E52" s="35"/>
+      <c r="H52" s="49"/>
       <c r="I52" s="13"/>
       <c r="J52" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="M52" s="42"/>
+      <c r="M52" s="49"/>
       <c r="N52" s="13"/>
       <c r="O52" s="13"/>
     </row>
@@ -1999,14 +1996,14 @@
       <c r="C53" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="49" t="s">
+      <c r="D53" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="E53" s="49"/>
-      <c r="H53" s="42"/>
+      <c r="E53" s="35"/>
+      <c r="H53" s="49"/>
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
-      <c r="M53" s="32" t="s">
+      <c r="M53" s="55" t="s">
         <v>81</v>
       </c>
       <c r="N53" s="13"/>
@@ -2015,7 +2012,7 @@
       </c>
     </row>
     <row r="54" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="59" t="s">
+      <c r="C54" s="36" t="s">
         <v>10</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -2024,27 +2021,27 @@
       <c r="E54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M54" s="32"/>
+      <c r="M54" s="55"/>
       <c r="N54" s="13"/>
       <c r="O54" s="13"/>
     </row>
     <row r="55" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C55" s="59"/>
+      <c r="C55" s="36"/>
       <c r="D55" s="13" t="s">
         <v>83</v>
       </c>
       <c r="E55" s="13"/>
-      <c r="M55" s="32"/>
+      <c r="M55" s="55"/>
       <c r="N55" s="13"/>
       <c r="O55" s="13"/>
     </row>
     <row r="56" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="59"/>
+      <c r="C56" s="36"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="M56" s="60" t="s">
+      <c r="M56" s="56" t="s">
         <v>85</v>
       </c>
       <c r="N56" s="13"/>
@@ -2053,17 +2050,17 @@
       </c>
     </row>
     <row r="57" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C57" s="59"/>
+      <c r="C57" s="36"/>
       <c r="D57" s="13" t="s">
         <v>86</v>
       </c>
       <c r="E57" s="10"/>
-      <c r="M57" s="60"/>
+      <c r="M57" s="56"/>
       <c r="N57" s="13"/>
       <c r="O57" s="13"/>
     </row>
     <row r="58" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="64" t="s">
+      <c r="C58" s="46" t="s">
         <v>87</v>
       </c>
       <c r="D58" s="13" t="s">
@@ -2073,13 +2070,13 @@
       <c r="H58" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I58" s="49" t="s">
+      <c r="I58" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="J58" s="49"/>
+      <c r="J58" s="35"/>
     </row>
     <row r="59" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C59" s="64"/>
+      <c r="C59" s="46"/>
       <c r="D59" s="13"/>
       <c r="E59" s="13" t="s">
         <v>139</v>
@@ -2087,13 +2084,13 @@
       <c r="H59" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I59" s="49" t="s">
+      <c r="I59" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="J59" s="49"/>
+      <c r="J59" s="35"/>
     </row>
     <row r="60" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C60" s="64"/>
+      <c r="C60" s="46"/>
       <c r="D60" s="13"/>
       <c r="E60" s="13" t="s">
         <v>140</v>
@@ -2101,16 +2098,16 @@
       <c r="H60" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I60" s="49" t="s">
+      <c r="I60" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="J60" s="49"/>
+      <c r="J60" s="35"/>
     </row>
     <row r="61" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="64"/>
+      <c r="C61" s="46"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
-      <c r="H61" s="48" t="s">
+      <c r="H61" s="29" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="2" t="s">
@@ -2122,42 +2119,42 @@
       <c r="M61" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N61" s="49" t="s">
+      <c r="N61" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="O61" s="49"/>
+      <c r="O61" s="35"/>
     </row>
     <row r="62" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H62" s="48"/>
+      <c r="H62" s="29"/>
       <c r="I62" s="13"/>
-      <c r="J62" s="30" t="s">
+      <c r="J62" s="38" t="s">
         <v>145</v>
       </c>
       <c r="M62" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N62" s="49" t="s">
+      <c r="N62" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="O62" s="49"/>
+      <c r="O62" s="35"/>
     </row>
     <row r="63" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H63" s="48"/>
+      <c r="H63" s="29"/>
       <c r="I63" s="13"/>
-      <c r="J63" s="31"/>
+      <c r="J63" s="47"/>
       <c r="M63" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N63" s="49" t="s">
+      <c r="N63" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="O63" s="49"/>
+      <c r="O63" s="35"/>
     </row>
     <row r="64" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H64" s="48"/>
+      <c r="H64" s="29"/>
       <c r="I64" s="13"/>
-      <c r="J64" s="31"/>
-      <c r="M64" s="59" t="s">
+      <c r="J64" s="47"/>
+      <c r="M64" s="36" t="s">
         <v>10</v>
       </c>
       <c r="N64" s="2" t="s">
@@ -2168,10 +2165,10 @@
       </c>
     </row>
     <row r="65" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H65" s="48"/>
+      <c r="H65" s="29"/>
       <c r="I65" s="13"/>
-      <c r="J65" s="65"/>
-      <c r="M65" s="71"/>
+      <c r="J65" s="39"/>
+      <c r="M65" s="37"/>
       <c r="N65" s="13" t="s">
         <v>150</v>
       </c>
@@ -2181,14 +2178,14 @@
       <c r="C66" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D66" s="49" t="s">
+      <c r="D66" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="E66" s="49"/>
-      <c r="H66" s="48"/>
+      <c r="E66" s="35"/>
+      <c r="H66" s="29"/>
       <c r="I66" s="13"/>
       <c r="J66" s="13"/>
-      <c r="M66" s="71"/>
+      <c r="M66" s="37"/>
       <c r="N66" s="13"/>
       <c r="O66" s="13" t="s">
         <v>151</v>
@@ -2198,18 +2195,18 @@
       <c r="C67" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="49" t="s">
+      <c r="D67" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E67" s="49"/>
-      <c r="H67" s="48"/>
-      <c r="I67" s="30"/>
-      <c r="J67" s="66" t="s">
+      <c r="E67" s="35"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="38"/>
+      <c r="J67" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="M67" s="71"/>
+      <c r="M67" s="37"/>
       <c r="N67" s="13"/>
-      <c r="O67" s="30" t="s">
+      <c r="O67" s="38" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2217,19 +2214,19 @@
       <c r="C68" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="49" t="s">
+      <c r="D68" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="E68" s="49"/>
-      <c r="H68" s="48"/>
-      <c r="I68" s="31"/>
-      <c r="J68" s="67"/>
-      <c r="M68" s="71"/>
+      <c r="E68" s="35"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="47"/>
+      <c r="J68" s="48"/>
+      <c r="M68" s="37"/>
       <c r="N68" s="13"/>
-      <c r="O68" s="65"/>
+      <c r="O68" s="39"/>
     </row>
     <row r="69" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C69" s="48" t="s">
+      <c r="C69" s="29" t="s">
         <v>10</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -2238,90 +2235,90 @@
       <c r="E69" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="59"/>
-      <c r="I69" s="31"/>
-      <c r="J69" s="67"/>
-      <c r="M69" s="72" t="s">
+      <c r="H69" s="36"/>
+      <c r="I69" s="47"/>
+      <c r="J69" s="48"/>
+      <c r="M69" s="40" t="s">
         <v>132</v>
       </c>
       <c r="N69" s="10"/>
-      <c r="O69" s="61" t="s">
+      <c r="O69" s="41" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="70" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="48"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="30" t="s">
+      <c r="C70" s="29"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="H70" s="42" t="s">
+      <c r="H70" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="I70" s="29"/>
-      <c r="J70" s="39" t="s">
+      <c r="I70" s="32"/>
+      <c r="J70" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="M70" s="72"/>
+      <c r="M70" s="40"/>
       <c r="N70" s="10"/>
-      <c r="O70" s="61"/>
+      <c r="O70" s="41"/>
     </row>
     <row r="71" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C71" s="48"/>
-      <c r="D71" s="65"/>
-      <c r="E71" s="65"/>
-      <c r="H71" s="42"/>
-      <c r="I71" s="29"/>
-      <c r="J71" s="39"/>
-      <c r="M71" s="72"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="39"/>
+      <c r="H71" s="49"/>
+      <c r="I71" s="32"/>
+      <c r="J71" s="50"/>
+      <c r="M71" s="40"/>
       <c r="N71" s="10"/>
-      <c r="O71" s="33" t="s">
+      <c r="O71" s="42" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="72" spans="3:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C72" s="48"/>
+      <c r="C72" s="29"/>
       <c r="D72" s="15" t="s">
         <v>92</v>
       </c>
       <c r="E72" s="11"/>
-      <c r="H72" s="42"/>
-      <c r="I72" s="29"/>
-      <c r="J72" s="39"/>
-      <c r="M72" s="72"/>
+      <c r="H72" s="49"/>
+      <c r="I72" s="32"/>
+      <c r="J72" s="50"/>
+      <c r="M72" s="40"/>
       <c r="N72" s="10"/>
-      <c r="O72" s="33"/>
+      <c r="O72" s="42"/>
     </row>
     <row r="73" spans="3:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C73" s="48"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30" t="s">
+      <c r="C73" s="29"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="H73" s="42"/>
-      <c r="I73" s="75"/>
+      <c r="H73" s="49"/>
+      <c r="I73" s="4"/>
       <c r="J73" s="21"/>
-      <c r="M73" s="72"/>
+      <c r="M73" s="40"/>
       <c r="N73" s="10" t="s">
         <v>135</v>
       </c>
       <c r="O73" s="10"/>
     </row>
     <row r="74" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C74" s="48"/>
-      <c r="D74" s="65"/>
-      <c r="E74" s="65"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="39"/>
       <c r="H74" s="26"/>
       <c r="I74" s="27"/>
       <c r="J74" s="25"/>
-      <c r="M74" s="72"/>
+      <c r="M74" s="40"/>
       <c r="N74" s="10"/>
       <c r="O74" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="75" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C75" s="48"/>
+      <c r="C75" s="29"/>
       <c r="D75" s="15" t="s">
         <v>94</v>
       </c>
@@ -2329,14 +2326,14 @@
       <c r="H75" s="26"/>
       <c r="I75" s="27"/>
       <c r="J75" s="25"/>
-      <c r="M75" s="72"/>
+      <c r="M75" s="40"/>
       <c r="N75" s="10"/>
       <c r="O75" s="10" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="76" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="48"/>
+      <c r="C76" s="29"/>
       <c r="D76" s="15"/>
       <c r="E76" s="14" t="s">
         <v>95</v>
@@ -2344,60 +2341,60 @@
       <c r="H76" s="26"/>
       <c r="I76" s="28"/>
       <c r="J76" s="27"/>
-      <c r="M76" s="73" t="s">
+      <c r="M76" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="N76" s="40"/>
-      <c r="O76" s="61" t="s">
+      <c r="N76" s="44"/>
+      <c r="O76" s="41" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="77" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C77" s="48"/>
+      <c r="C77" s="29"/>
       <c r="D77" s="15"/>
-      <c r="E77" s="61" t="s">
+      <c r="E77" s="41" t="s">
         <v>96</v>
       </c>
       <c r="H77" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I77" s="49" t="s">
+      <c r="I77" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="J77" s="49"/>
-      <c r="M77" s="73"/>
-      <c r="N77" s="41"/>
-      <c r="O77" s="61"/>
+      <c r="J77" s="35"/>
+      <c r="M77" s="43"/>
+      <c r="N77" s="45"/>
+      <c r="O77" s="41"/>
     </row>
     <row r="78" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="48"/>
+      <c r="C78" s="29"/>
       <c r="D78" s="15"/>
-      <c r="E78" s="61"/>
+      <c r="E78" s="41"/>
       <c r="H78" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I78" s="49" t="s">
+      <c r="I78" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="J78" s="49"/>
+      <c r="J78" s="35"/>
     </row>
     <row r="79" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="48"/>
+      <c r="C79" s="29"/>
       <c r="D79" s="15"/>
-      <c r="E79" s="61"/>
+      <c r="E79" s="41"/>
       <c r="H79" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I79" s="49"/>
-      <c r="J79" s="49"/>
+      <c r="I79" s="35"/>
+      <c r="J79" s="35"/>
     </row>
     <row r="80" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="48"/>
-      <c r="D80" s="61" t="s">
+      <c r="C80" s="29"/>
+      <c r="D80" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="E80" s="62"/>
-      <c r="H80" s="48" t="s">
+      <c r="E80" s="72"/>
+      <c r="H80" s="29" t="s">
         <v>10</v>
       </c>
       <c r="I80" s="2" t="s">
@@ -2409,46 +2406,46 @@
       <c r="M80" s="16"/>
     </row>
     <row r="81" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C81" s="48"/>
-      <c r="D81" s="61"/>
-      <c r="E81" s="63"/>
-      <c r="H81" s="48"/>
-      <c r="I81" s="66" t="s">
+      <c r="C81" s="29"/>
+      <c r="D81" s="41"/>
+      <c r="E81" s="73"/>
+      <c r="H81" s="29"/>
+      <c r="I81" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="J81" s="29"/>
+      <c r="J81" s="32"/>
       <c r="M81" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N81" s="49" t="s">
+      <c r="N81" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="O81" s="49"/>
+      <c r="O81" s="35"/>
     </row>
     <row r="82" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C82" s="48"/>
+      <c r="C82" s="29"/>
       <c r="D82" s="11" t="s">
         <v>98</v>
       </c>
       <c r="E82" s="11"/>
-      <c r="H82" s="48"/>
-      <c r="I82" s="74"/>
-      <c r="J82" s="29"/>
+      <c r="H82" s="29"/>
+      <c r="I82" s="31"/>
+      <c r="J82" s="32"/>
       <c r="M82" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N82" s="49" t="s">
+      <c r="N82" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="O82" s="49"/>
+      <c r="O82" s="35"/>
     </row>
     <row r="83" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C83" s="48"/>
+      <c r="C83" s="29"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="H83" s="48"/>
+      <c r="H83" s="29"/>
       <c r="I83" s="13"/>
       <c r="J83" s="23" t="s">
         <v>158</v>
@@ -2456,23 +2453,23 @@
       <c r="M83" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N83" s="49" t="s">
+      <c r="N83" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="O83" s="49"/>
+      <c r="O83" s="35"/>
     </row>
     <row r="84" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C84" s="48"/>
+      <c r="C84" s="29"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H84" s="48"/>
+      <c r="H84" s="29"/>
       <c r="I84" s="13"/>
-      <c r="J84" s="29" t="s">
+      <c r="J84" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="M84" s="48" t="s">
+      <c r="M84" s="29" t="s">
         <v>10</v>
       </c>
       <c r="N84" s="2" t="s">
@@ -2483,106 +2480,106 @@
       </c>
     </row>
     <row r="85" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C85" s="48"/>
+      <c r="C85" s="29"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="H85" s="48"/>
+      <c r="H85" s="29"/>
       <c r="I85" s="13"/>
-      <c r="J85" s="29"/>
-      <c r="M85" s="48"/>
+      <c r="J85" s="32"/>
+      <c r="M85" s="29"/>
       <c r="N85" s="13" t="s">
         <v>150</v>
       </c>
       <c r="O85" s="13"/>
     </row>
     <row r="86" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C86" s="48"/>
-      <c r="D86" s="44"/>
-      <c r="E86" s="61" t="s">
+      <c r="C86" s="29"/>
+      <c r="D86" s="68"/>
+      <c r="E86" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="H86" s="48"/>
-      <c r="I86" s="30"/>
-      <c r="J86" s="29"/>
-      <c r="M86" s="48"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="38"/>
+      <c r="J86" s="32"/>
+      <c r="M86" s="29"/>
       <c r="N86" s="13"/>
       <c r="O86" s="13" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="87" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="48"/>
-      <c r="D87" s="45"/>
-      <c r="E87" s="61"/>
-      <c r="H87" s="48"/>
-      <c r="I87" s="31"/>
-      <c r="J87" s="29"/>
-      <c r="M87" s="48"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="69"/>
+      <c r="E87" s="41"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="47"/>
+      <c r="J87" s="32"/>
+      <c r="M87" s="29"/>
       <c r="N87" s="13"/>
-      <c r="O87" s="61" t="s">
+      <c r="O87" s="41" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="88" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C88" s="48"/>
+      <c r="C88" s="29"/>
       <c r="D88" s="11" t="s">
         <v>113</v>
       </c>
       <c r="E88" s="11"/>
-      <c r="H88" s="48"/>
-      <c r="I88" s="31"/>
-      <c r="J88" s="29"/>
-      <c r="M88" s="48"/>
+      <c r="H88" s="29"/>
+      <c r="I88" s="47"/>
+      <c r="J88" s="32"/>
+      <c r="M88" s="29"/>
       <c r="N88" s="13"/>
-      <c r="O88" s="61"/>
+      <c r="O88" s="41"/>
     </row>
     <row r="89" spans="3:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C89" s="48"/>
+      <c r="C89" s="29"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="H89" s="68" t="s">
+      <c r="H89" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="I89" s="69"/>
-      <c r="J89" s="29" t="s">
+      <c r="I89" s="33"/>
+      <c r="J89" s="32" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="90" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C90" s="42" t="s">
+      <c r="C90" s="49" t="s">
         <v>110</v>
       </c>
       <c r="D90" s="20"/>
       <c r="E90" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="H90" s="68"/>
-      <c r="I90" s="70"/>
-      <c r="J90" s="29"/>
+      <c r="H90" s="74"/>
+      <c r="I90" s="34"/>
+      <c r="J90" s="32"/>
     </row>
     <row r="91" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C91" s="42"/>
+      <c r="C91" s="49"/>
       <c r="D91" s="20"/>
       <c r="E91" s="21" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="92" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C92" s="42"/>
+      <c r="C92" s="49"/>
       <c r="D92" s="20"/>
       <c r="E92" s="21"/>
     </row>
     <row r="93" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C93" s="42"/>
+      <c r="C93" s="49"/>
       <c r="D93" s="20"/>
       <c r="E93" s="21"/>
     </row>
     <row r="94" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C94" s="42" t="s">
+      <c r="C94" s="49" t="s">
         <v>102</v>
       </c>
       <c r="D94" s="20"/>
@@ -2591,52 +2588,52 @@
       </c>
     </row>
     <row r="95" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C95" s="42"/>
+      <c r="C95" s="49"/>
       <c r="D95" s="20"/>
       <c r="E95" s="21" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="96" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C96" s="42"/>
+      <c r="C96" s="49"/>
       <c r="D96" s="20"/>
       <c r="E96" s="21"/>
     </row>
     <row r="97" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C97" s="42"/>
+      <c r="C97" s="49"/>
       <c r="D97" s="20"/>
       <c r="E97" s="21"/>
     </row>
     <row r="98" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C98" s="43" t="s">
+      <c r="C98" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="D98" s="44"/>
-      <c r="E98" s="46" t="s">
+      <c r="D98" s="68"/>
+      <c r="E98" s="70" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="99" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C99" s="43"/>
-      <c r="D99" s="45"/>
-      <c r="E99" s="47"/>
+      <c r="C99" s="67"/>
+      <c r="D99" s="69"/>
+      <c r="E99" s="71"/>
     </row>
     <row r="100" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C100" s="43"/>
+      <c r="C100" s="67"/>
       <c r="D100" s="20"/>
       <c r="E100" s="21" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="101" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C101" s="43"/>
+      <c r="C101" s="67"/>
       <c r="D101" s="20"/>
       <c r="E101" s="21" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="102" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C102" s="36" t="s">
+      <c r="C102" s="64" t="s">
         <v>115</v>
       </c>
       <c r="D102" s="20"/>
@@ -2645,86 +2642,86 @@
       </c>
     </row>
     <row r="103" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C103" s="37"/>
+      <c r="C103" s="65"/>
       <c r="D103" s="20"/>
       <c r="E103" s="22"/>
       <c r="J103" s="16"/>
     </row>
     <row r="104" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C104" s="38"/>
+      <c r="C104" s="66"/>
       <c r="D104" s="20"/>
       <c r="E104" s="21"/>
     </row>
     <row r="105" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C105" s="36" t="s">
+      <c r="C105" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="D105" s="29" t="s">
+      <c r="D105" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="E105" s="39"/>
+      <c r="E105" s="50"/>
     </row>
     <row r="106" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C106" s="37"/>
-      <c r="D106" s="29"/>
-      <c r="E106" s="39"/>
+      <c r="C106" s="65"/>
+      <c r="D106" s="32"/>
+      <c r="E106" s="50"/>
     </row>
     <row r="107" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C107" s="37"/>
+      <c r="C107" s="65"/>
       <c r="D107" s="20"/>
       <c r="E107" s="21" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="108" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C108" s="37"/>
-      <c r="D108" s="40"/>
-      <c r="E108" s="33" t="s">
+      <c r="C108" s="65"/>
+      <c r="D108" s="44"/>
+      <c r="E108" s="42" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="109" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C109" s="37"/>
-      <c r="D109" s="41"/>
-      <c r="E109" s="33"/>
+      <c r="C109" s="65"/>
+      <c r="D109" s="45"/>
+      <c r="E109" s="42"/>
     </row>
     <row r="110" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C110" s="37"/>
+      <c r="C110" s="65"/>
       <c r="D110" s="10" t="s">
         <v>120</v>
       </c>
       <c r="E110" s="10"/>
     </row>
     <row r="111" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C111" s="38"/>
+      <c r="C111" s="66"/>
       <c r="D111" s="10"/>
       <c r="E111" s="10" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="112" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C112" s="32" t="s">
+      <c r="C112" s="55" t="s">
         <v>123</v>
       </c>
       <c r="D112" s="13"/>
-      <c r="E112" s="33" t="s">
+      <c r="E112" s="42" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="113" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C113" s="32"/>
+      <c r="C113" s="55"/>
       <c r="D113" s="13"/>
-      <c r="E113" s="33"/>
+      <c r="E113" s="42"/>
     </row>
     <row r="114" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C114" s="32"/>
+      <c r="C114" s="55"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="115" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C115" s="34" t="s">
+      <c r="C115" s="62" t="s">
         <v>127</v>
       </c>
       <c r="D115" s="13"/>
@@ -2733,22 +2730,135 @@
       </c>
     </row>
     <row r="116" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C116" s="35"/>
+      <c r="C116" s="63"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
     <row r="117" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C117" s="35"/>
+      <c r="C117" s="63"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
     <row r="118" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C118" s="35"/>
+      <c r="C118" s="63"/>
       <c r="D118" s="10"/>
       <c r="E118" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="137">
+    <mergeCell ref="I86:I88"/>
+    <mergeCell ref="C112:C114"/>
+    <mergeCell ref="E112:E113"/>
+    <mergeCell ref="C115:C118"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="C105:C111"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="C69:C89"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="E77:E79"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="H89:H90"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="H7:H13"/>
+    <mergeCell ref="M7:M19"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="N10:N12"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M20:M24"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="H23:H27"/>
+    <mergeCell ref="M25:M29"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="H28:H32"/>
+    <mergeCell ref="I28:I32"/>
+    <mergeCell ref="J28:J32"/>
+    <mergeCell ref="M30:M34"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="D42:D46"/>
+    <mergeCell ref="E42:E46"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="H46:H50"/>
+    <mergeCell ref="M46:M49"/>
+    <mergeCell ref="M50:M52"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="M53:M55"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="M56:M57"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="H61:H69"/>
+    <mergeCell ref="J62:J65"/>
+    <mergeCell ref="I67:I69"/>
+    <mergeCell ref="J67:J69"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="I70:I72"/>
+    <mergeCell ref="J70:J72"/>
     <mergeCell ref="H80:H88"/>
     <mergeCell ref="I81:I82"/>
     <mergeCell ref="J81:J82"/>
@@ -2772,120 +2882,7 @@
     <mergeCell ref="O87:O88"/>
     <mergeCell ref="I78:J78"/>
     <mergeCell ref="I79:J79"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="H61:H69"/>
-    <mergeCell ref="J62:J65"/>
-    <mergeCell ref="I67:I69"/>
-    <mergeCell ref="J67:J69"/>
-    <mergeCell ref="H70:H73"/>
-    <mergeCell ref="I70:I72"/>
-    <mergeCell ref="J70:J72"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="C37:C41"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="D42:D46"/>
-    <mergeCell ref="E42:E46"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="H46:H50"/>
-    <mergeCell ref="M46:M49"/>
-    <mergeCell ref="M50:M52"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="M53:M55"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="M56:M57"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="M25:M29"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="H28:H32"/>
-    <mergeCell ref="I28:I32"/>
-    <mergeCell ref="J28:J32"/>
-    <mergeCell ref="M30:M34"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="O30:O32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M20:M24"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="H7:H13"/>
-    <mergeCell ref="M7:M19"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="N10:N12"/>
-    <mergeCell ref="O10:O12"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="N6:O6"/>
     <mergeCell ref="J84:J88"/>
-    <mergeCell ref="I86:I88"/>
-    <mergeCell ref="C112:C114"/>
-    <mergeCell ref="E112:E113"/>
-    <mergeCell ref="C115:C118"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="C105:C111"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="C69:C89"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="E77:E79"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="H89:H90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
novo diagrama Ver loja mais perto
</commit_message>
<xml_diff>
--- a/projeto/Especificação de Use Cases.XLSX
+++ b/projeto/Especificação de Use Cases.XLSX
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CésarAugustodaCostaB\Documents\Projects\LI4\projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guilhermeviveiros/Desktop/Documentos/2-semestre/LI4/projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719D4615-71B7-48E8-B7BA-666F810CEDB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3928A98-3B4F-4941-B130-6B919A8EEF98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="164">
   <si>
     <t>Use Case:</t>
   </si>
@@ -378,24 +378,12 @@
     <t>13.1 Termina Confecionar receita</t>
   </si>
   <si>
-    <t xml:space="preserve">7.1 Indica o conceito a questionar </t>
-  </si>
-  <si>
-    <t>7.2 Procura conceito</t>
-  </si>
-  <si>
-    <t>7.3 Apresenta a descrição, uma imagem e/ou vídeo sobre o conceito</t>
-  </si>
-  <si>
     <t>7.4 Volta à confeção</t>
   </si>
   <si>
     <t>7.5 Volta ao passo 7</t>
   </si>
   <si>
-    <t>Comportamento Alternativo 5[Ator questiona sistema sobre um conceito (técnica, ingrediente ou utensílio) culinário](passo 7)</t>
-  </si>
-  <si>
     <t>Exceção 1[Não confirma](passo 2 ou 4)</t>
   </si>
   <si>
@@ -519,25 +507,16 @@
     <t>foi encontrada uma loja</t>
   </si>
   <si>
-    <t>1. Solicita ver a loja mais perto</t>
-  </si>
-  <si>
-    <t>2. Recebe localização do cliente</t>
-  </si>
-  <si>
-    <t>3. Calcula a loja mais perto das conhecidas</t>
-  </si>
-  <si>
-    <t>4. Mostra loja</t>
-  </si>
-  <si>
-    <t>Exceção 1 [Não é possivel obter a localização do utilizador] (passo 4)</t>
-  </si>
-  <si>
-    <t>2.1 Informa que deve permitir ao sistema conhecer a sua localização</t>
-  </si>
-  <si>
     <t>Estar autenticado, existem lojas</t>
+  </si>
+  <si>
+    <t>1. Solicita ver a loja mais perto de uma determinada localização</t>
+  </si>
+  <si>
+    <t>2. Calcula a loja mais perto das conhecidas</t>
+  </si>
+  <si>
+    <t>3.Mostra loja</t>
   </si>
 </sst>
 </file>
@@ -702,7 +681,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -774,17 +753,123 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -801,21 +886,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -831,97 +901,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1304,101 +1289,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:O118"/>
+  <dimension ref="C4:O114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="61" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M100" sqref="M100"/>
+    <sheetView tabSelected="1" topLeftCell="G91" zoomScale="221" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="1" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="7" width="8.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" customWidth="1"/>
-    <col min="15" max="15" width="22.140625" customWidth="1"/>
-    <col min="16" max="1025" width="8.42578125" customWidth="1"/>
+    <col min="6" max="7" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" customWidth="1"/>
+    <col min="10" max="10" width="23.1640625" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" customWidth="1"/>
+    <col min="14" max="14" width="23.5" customWidth="1"/>
+    <col min="15" max="15" width="22.1640625" customWidth="1"/>
+    <col min="16" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="52"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="52" t="s">
+      <c r="I4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="52"/>
+      <c r="J4" s="32"/>
       <c r="M4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="52" t="s">
+      <c r="N4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="52"/>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O4" s="32"/>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="52"/>
+      <c r="E5" s="32"/>
       <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="52" t="s">
+      <c r="I5" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="52"/>
+      <c r="J5" s="32"/>
       <c r="M5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="52" t="s">
+      <c r="N5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="52"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O5" s="32"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="52" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="52"/>
+      <c r="D6" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="32"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="52" t="s">
+      <c r="I6" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="52"/>
+      <c r="J6" s="32"/>
       <c r="M6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="52" t="s">
+      <c r="N6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="52"/>
-    </row>
-    <row r="7" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="48" t="s">
+      <c r="O6" s="32"/>
+    </row>
+    <row r="7" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="52" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1407,7 +1392,7 @@
       <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="52" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1416,7 +1401,7 @@
       <c r="J7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="48" t="s">
+      <c r="M7" s="52" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="2" t="s">
@@ -1426,102 +1411,102 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="48"/>
+    <row r="8" spans="3:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="C8" s="52"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="H8" s="48"/>
+      <c r="H8" s="52"/>
       <c r="I8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="M8" s="48"/>
+      <c r="M8" s="52"/>
       <c r="N8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="48"/>
+    <row r="9" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="52"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="48"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="55" t="s">
+      <c r="H9" s="52"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="48"/>
+      <c r="M9" s="52"/>
       <c r="N9" s="3"/>
       <c r="O9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="48"/>
+    <row r="10" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="52"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="48"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="56" t="s">
+      <c r="H10" s="52"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="64"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="67"/>
+      <c r="O10" s="66" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="48"/>
+    <row r="11" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C11" s="52"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="48"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="55"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="56"/>
-    </row>
-    <row r="12" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="42" t="s">
+      <c r="H11" s="52"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="64"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="66"/>
+    </row>
+    <row r="12" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="56" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="55" t="s">
+      <c r="H12" s="52"/>
+      <c r="I12" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="54"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="56"/>
-    </row>
-    <row r="13" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="42"/>
+      <c r="J12" s="67"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="66"/>
+    </row>
+    <row r="13" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="56"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="48"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="54"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="56" t="s">
+      <c r="H13" s="52"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="67"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="66" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="42"/>
+    <row r="14" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C14" s="56"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
         <v>27</v>
@@ -1529,11 +1514,11 @@
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="56"/>
-    </row>
-    <row r="15" spans="3:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="M14" s="52"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="66"/>
+    </row>
+    <row r="15" spans="3:15" ht="48" x14ac:dyDescent="0.2">
       <c r="C15" s="7" t="s">
         <v>28</v>
       </c>
@@ -1544,101 +1529,101 @@
       <c r="H15" s="8"/>
       <c r="I15" s="6"/>
       <c r="J15" s="9"/>
-      <c r="M15" s="48"/>
+      <c r="M15" s="52"/>
       <c r="N15" s="4" t="s">
         <v>30</v>
       </c>
       <c r="O15" s="10"/>
     </row>
-    <row r="16" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M16" s="48"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="56" t="s">
+    <row r="16" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M16" s="52"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="66" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M17" s="48"/>
-      <c r="N17" s="57"/>
-      <c r="O17" s="56"/>
-    </row>
-    <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M18" s="48"/>
-      <c r="N18" s="56" t="s">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="M17" s="52"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="66"/>
+    </row>
+    <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M18" s="52"/>
+      <c r="N18" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="O18" s="57"/>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M19" s="48"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="57"/>
-    </row>
-    <row r="20" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O18" s="68"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="M19" s="52"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="68"/>
+    </row>
+    <row r="20" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="52" t="s">
+      <c r="D20" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="52"/>
+      <c r="E20" s="32"/>
       <c r="H20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I20" s="52" t="s">
+      <c r="I20" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="52"/>
-      <c r="M20" s="42" t="s">
+      <c r="J20" s="32"/>
+      <c r="M20" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="N20" s="55" t="s">
+      <c r="N20" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="O20" s="58"/>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O20" s="65"/>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="52" t="s">
+      <c r="D21" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="52"/>
+      <c r="E21" s="32"/>
       <c r="H21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="52" t="s">
+      <c r="I21" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="52"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="58"/>
-    </row>
-    <row r="22" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="32"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="64"/>
+      <c r="O21" s="65"/>
+    </row>
+    <row r="22" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="52"/>
+      <c r="E22" s="32"/>
       <c r="H22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="52" t="s">
+      <c r="I22" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="J22" s="52"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="56" t="s">
+      <c r="J22" s="32"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="65"/>
+      <c r="O22" s="66" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="59" t="s">
+    <row r="23" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="58" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1647,7 +1632,7 @@
       <c r="E23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="59" t="s">
+      <c r="H23" s="58" t="s">
         <v>10</v>
       </c>
       <c r="I23" s="2" t="s">
@@ -1656,165 +1641,165 @@
       <c r="J23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="42"/>
-      <c r="N23" s="58"/>
-      <c r="O23" s="56"/>
-    </row>
-    <row r="24" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C24" s="59"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="65"/>
+      <c r="O23" s="66"/>
+    </row>
+    <row r="24" spans="3:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="C24" s="58"/>
       <c r="D24" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="H24" s="59"/>
+      <c r="H24" s="58"/>
       <c r="I24" s="3" t="s">
         <v>41</v>
       </c>
       <c r="J24" s="3"/>
-      <c r="M24" s="42"/>
+      <c r="M24" s="56"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="59"/>
+    <row r="25" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="58"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="59"/>
+      <c r="H25" s="58"/>
       <c r="I25" s="10"/>
       <c r="J25" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="M25" s="42" t="s">
+      <c r="M25" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="55" t="s">
+      <c r="N25" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="O25" s="58"/>
-    </row>
-    <row r="26" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="59"/>
+      <c r="O25" s="65"/>
+    </row>
+    <row r="26" spans="3:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="C26" s="58"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H26" s="59"/>
+      <c r="H26" s="58"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="M26" s="42"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="58"/>
-    </row>
-    <row r="27" spans="3:15" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M26" s="56"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="65"/>
+    </row>
+    <row r="27" spans="3:15" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27" s="8"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="H27" s="59"/>
+      <c r="H27" s="58"/>
       <c r="I27" s="19"/>
       <c r="J27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M27" s="42"/>
-      <c r="N27" s="58"/>
-      <c r="O27" s="56" t="s">
+      <c r="M27" s="56"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="66" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H28" s="60" t="s">
+    <row r="28" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="I28" s="61"/>
-      <c r="J28" s="62" t="s">
+      <c r="I28" s="60"/>
+      <c r="J28" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="M28" s="42"/>
-      <c r="N28" s="58"/>
-      <c r="O28" s="56"/>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H29" s="60"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="62"/>
-      <c r="M29" s="42"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="65"/>
+      <c r="O28" s="66"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="H29" s="59"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="61"/>
+      <c r="M29" s="56"/>
       <c r="N29" s="11"/>
       <c r="O29" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H30" s="60"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="62"/>
-      <c r="M30" s="42" t="s">
+    <row r="30" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30" s="59"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="61"/>
+      <c r="M30" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="N30" s="54"/>
-      <c r="O30" s="54" t="s">
+      <c r="N30" s="67"/>
+      <c r="O30" s="67" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H31" s="60"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="62"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="54"/>
-      <c r="O31" s="54"/>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H32" s="60"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="62"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="54"/>
-      <c r="O32" s="54"/>
-    </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M33" s="42"/>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="H31" s="59"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="61"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="61"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="67"/>
+      <c r="O32" s="67"/>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="M33" s="56"/>
       <c r="N33" s="10"/>
       <c r="O33" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="52" t="s">
+      <c r="D34" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="52"/>
-      <c r="M34" s="42"/>
+      <c r="E34" s="32"/>
+      <c r="M34" s="56"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="52"/>
-    </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="E35" s="32"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="52" t="s">
+      <c r="D36" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="52"/>
-    </row>
-    <row r="37" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="59" t="s">
+      <c r="E36" s="32"/>
+    </row>
+    <row r="37" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="58" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -1824,105 +1809,105 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C38" s="59"/>
+    <row r="38" spans="3:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="C38" s="58"/>
       <c r="D38" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C39" s="59"/>
+    <row r="39" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C39" s="58"/>
       <c r="D39" s="10"/>
       <c r="E39" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C40" s="59"/>
+    <row r="40" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C40" s="58"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C41" s="59"/>
+    <row r="41" spans="3:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="C41" s="58"/>
       <c r="D41" s="17"/>
       <c r="E41" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="3:15" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="60" t="s">
+    <row r="42" spans="3:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="61"/>
-      <c r="E42" s="62" t="s">
+      <c r="D42" s="60"/>
+      <c r="E42" s="61" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="60"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="62"/>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C43" s="59"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="61"/>
       <c r="H43" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I43" s="52" t="s">
+      <c r="I43" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="J43" s="52"/>
+      <c r="J43" s="32"/>
       <c r="M43" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N43" s="52" t="s">
+      <c r="N43" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="O43" s="52"/>
-    </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="60"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="62"/>
+      <c r="O43" s="32"/>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C44" s="59"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="61"/>
       <c r="H44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I44" s="52" t="s">
+      <c r="I44" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="J44" s="52"/>
+      <c r="J44" s="32"/>
       <c r="M44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N44" s="52" t="s">
+      <c r="N44" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="O44" s="52"/>
-    </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="60"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="62"/>
+      <c r="O44" s="32"/>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C45" s="59"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="61"/>
       <c r="H45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I45" s="52" t="s">
+      <c r="I45" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="J45" s="52"/>
+      <c r="J45" s="32"/>
       <c r="M45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N45" s="52" t="s">
+      <c r="N45" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="O45" s="52"/>
-    </row>
-    <row r="46" spans="3:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="60"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="62"/>
-      <c r="H46" s="48" t="s">
+      <c r="O45" s="32"/>
+    </row>
+    <row r="46" spans="3:15" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="59"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="61"/>
+      <c r="H46" s="52" t="s">
         <v>10</v>
       </c>
       <c r="I46" s="2" t="s">
@@ -1931,7 +1916,7 @@
       <c r="J46" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M46" s="63" t="s">
+      <c r="M46" s="38" t="s">
         <v>10</v>
       </c>
       <c r="N46" s="2" t="s">
@@ -1941,49 +1926,49 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="3:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="H47" s="48"/>
+    <row r="47" spans="3:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="H47" s="52"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="M47" s="63"/>
+      <c r="M47" s="38"/>
       <c r="N47" s="13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O47" s="13"/>
     </row>
-    <row r="48" spans="3:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="H48" s="48"/>
+    <row r="48" spans="3:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="H48" s="52"/>
       <c r="I48" s="13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J48" s="13"/>
-      <c r="M48" s="63"/>
+      <c r="M48" s="38"/>
       <c r="N48" s="13"/>
       <c r="O48" s="13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H49" s="48"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="H49" s="52"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="M49" s="63"/>
+      <c r="M49" s="38"/>
       <c r="N49" s="13"/>
       <c r="O49" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H50" s="48"/>
+    <row r="50" spans="3:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H50" s="52"/>
       <c r="I50" s="13"/>
       <c r="J50" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="M50" s="42" t="s">
+      <c r="M50" s="56" t="s">
         <v>73</v>
       </c>
       <c r="N50" s="13"/>
@@ -1991,56 +1976,56 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C51" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D51" s="52" t="s">
+      <c r="D51" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="E51" s="52"/>
-      <c r="H51" s="42" t="s">
+      <c r="E51" s="32"/>
+      <c r="H51" s="56" t="s">
         <v>76</v>
       </c>
       <c r="I51" s="13"/>
       <c r="J51" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M51" s="42"/>
+      <c r="M51" s="56"/>
       <c r="N51" s="13"/>
       <c r="O51" s="13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:15" ht="16" x14ac:dyDescent="0.2">
       <c r="C52" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="52" t="s">
+      <c r="D52" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="52"/>
-      <c r="H52" s="42"/>
+      <c r="E52" s="32"/>
+      <c r="H52" s="56"/>
       <c r="I52" s="13"/>
       <c r="J52" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="M52" s="42"/>
+      <c r="M52" s="56"/>
       <c r="N52" s="13"/>
       <c r="O52" s="13"/>
     </row>
-    <row r="53" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C53" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="52" t="s">
+      <c r="D53" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="E53" s="52"/>
-      <c r="H53" s="42"/>
+      <c r="E53" s="32"/>
+      <c r="H53" s="56"/>
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
-      <c r="M53" s="31" t="s">
+      <c r="M53" s="62" t="s">
         <v>81</v>
       </c>
       <c r="N53" s="13"/>
@@ -2048,8 +2033,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="63" t="s">
+    <row r="54" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="38" t="s">
         <v>10</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -2058,46 +2043,46 @@
       <c r="E54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M54" s="31"/>
+      <c r="M54" s="62"/>
       <c r="N54" s="13"/>
       <c r="O54" s="13"/>
     </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C55" s="63"/>
+    <row r="55" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C55" s="38"/>
       <c r="D55" s="13" t="s">
         <v>83</v>
       </c>
       <c r="E55" s="13"/>
-      <c r="M55" s="31"/>
+      <c r="M55" s="62"/>
       <c r="N55" s="13"/>
       <c r="O55" s="13"/>
     </row>
-    <row r="56" spans="3:15" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="63"/>
+    <row r="56" spans="3:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="38"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="M56" s="64" t="s">
+      <c r="M56" s="63" t="s">
         <v>85</v>
       </c>
       <c r="N56" s="13"/>
       <c r="O56" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C57" s="63"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C57" s="38"/>
       <c r="D57" s="13" t="s">
         <v>86</v>
       </c>
       <c r="E57" s="10"/>
-      <c r="M57" s="64"/>
+      <c r="M57" s="63"/>
       <c r="N57" s="13"/>
       <c r="O57" s="13"/>
     </row>
-    <row r="58" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="65" t="s">
+    <row r="58" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="53" t="s">
         <v>87</v>
       </c>
       <c r="D58" s="13" t="s">
@@ -2107,44 +2092,44 @@
       <c r="H58" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I58" s="52" t="s">
-        <v>128</v>
-      </c>
-      <c r="J58" s="52"/>
-    </row>
-    <row r="59" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C59" s="65"/>
+      <c r="I58" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="J58" s="32"/>
+    </row>
+    <row r="59" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C59" s="53"/>
       <c r="D59" s="13"/>
       <c r="E59" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H59" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I59" s="52" t="s">
+      <c r="I59" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="J59" s="52"/>
-    </row>
-    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C60" s="65"/>
+      <c r="J59" s="32"/>
+    </row>
+    <row r="60" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C60" s="53"/>
       <c r="D60" s="13"/>
       <c r="E60" s="13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H60" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I60" s="52" t="s">
-        <v>129</v>
-      </c>
-      <c r="J60" s="52"/>
-    </row>
-    <row r="61" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="65"/>
+      <c r="I60" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="J60" s="32"/>
+    </row>
+    <row r="61" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="53"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
-      <c r="H61" s="48" t="s">
+      <c r="H61" s="52" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="2" t="s">
@@ -2156,42 +2141,42 @@
       <c r="M61" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N61" s="52" t="s">
-        <v>148</v>
-      </c>
-      <c r="O61" s="52"/>
-    </row>
-    <row r="62" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H62" s="48"/>
+      <c r="N61" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="O61" s="32"/>
+    </row>
+    <row r="62" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="H62" s="52"/>
       <c r="I62" s="13"/>
-      <c r="J62" s="29" t="s">
-        <v>145</v>
+      <c r="J62" s="36" t="s">
+        <v>141</v>
       </c>
       <c r="M62" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N62" s="52" t="s">
+      <c r="N62" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="O62" s="52"/>
-    </row>
-    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H63" s="48"/>
+      <c r="O62" s="32"/>
+    </row>
+    <row r="63" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="H63" s="52"/>
       <c r="I63" s="13"/>
-      <c r="J63" s="30"/>
+      <c r="J63" s="54"/>
       <c r="M63" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N63" s="52" t="s">
-        <v>149</v>
-      </c>
-      <c r="O63" s="52"/>
-    </row>
-    <row r="64" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H64" s="48"/>
+      <c r="N63" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="O63" s="32"/>
+    </row>
+    <row r="64" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H64" s="52"/>
       <c r="I64" s="13"/>
-      <c r="J64" s="30"/>
-      <c r="M64" s="63" t="s">
+      <c r="J64" s="54"/>
+      <c r="M64" s="38" t="s">
         <v>10</v>
       </c>
       <c r="N64" s="2" t="s">
@@ -2201,69 +2186,69 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H65" s="48"/>
+    <row r="65" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="H65" s="52"/>
       <c r="I65" s="13"/>
-      <c r="J65" s="66"/>
-      <c r="M65" s="72"/>
+      <c r="J65" s="37"/>
+      <c r="M65" s="39"/>
       <c r="N65" s="13" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="O65" s="13"/>
     </row>
-    <row r="66" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:15" ht="16" x14ac:dyDescent="0.2">
       <c r="C66" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D66" s="52" t="s">
+      <c r="D66" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="E66" s="52"/>
-      <c r="H66" s="48"/>
+      <c r="E66" s="32"/>
+      <c r="H66" s="52"/>
       <c r="I66" s="13"/>
       <c r="J66" s="13"/>
-      <c r="M66" s="72"/>
+      <c r="M66" s="39"/>
       <c r="N66" s="13"/>
       <c r="O66" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="67" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C67" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="52" t="s">
+      <c r="D67" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E67" s="52"/>
-      <c r="H67" s="48"/>
-      <c r="I67" s="29"/>
-      <c r="J67" s="67" t="s">
-        <v>146</v>
-      </c>
-      <c r="M67" s="72"/>
+      <c r="E67" s="32"/>
+      <c r="H67" s="52"/>
+      <c r="I67" s="36"/>
+      <c r="J67" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="M67" s="39"/>
       <c r="N67" s="13"/>
-      <c r="O67" s="29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="68" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O67" s="36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C68" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="52" t="s">
+      <c r="D68" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="E68" s="52"/>
-      <c r="H68" s="48"/>
-      <c r="I68" s="30"/>
-      <c r="J68" s="68"/>
-      <c r="M68" s="72"/>
+      <c r="E68" s="32"/>
+      <c r="H68" s="52"/>
+      <c r="I68" s="54"/>
+      <c r="J68" s="55"/>
+      <c r="M68" s="39"/>
       <c r="N68" s="13"/>
-      <c r="O68" s="66"/>
-    </row>
-    <row r="69" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C69" s="48" t="s">
+      <c r="O68" s="37"/>
+    </row>
+    <row r="69" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C69" s="52" t="s">
         <v>10</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -2272,90 +2257,90 @@
       <c r="E69" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="63"/>
-      <c r="I69" s="30"/>
-      <c r="J69" s="68"/>
-      <c r="M69" s="73" t="s">
-        <v>132</v>
+      <c r="H69" s="38"/>
+      <c r="I69" s="54"/>
+      <c r="J69" s="55"/>
+      <c r="M69" s="46" t="s">
+        <v>128</v>
       </c>
       <c r="N69" s="10"/>
-      <c r="O69" s="49" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="70" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="48"/>
-      <c r="D70" s="29"/>
-      <c r="E70" s="29" t="s">
+      <c r="O69" s="47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C70" s="52"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="H70" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="I70" s="38"/>
-      <c r="J70" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="M70" s="73"/>
+      <c r="H70" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="I70" s="35"/>
+      <c r="J70" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="M70" s="46"/>
       <c r="N70" s="10"/>
-      <c r="O70" s="49"/>
-    </row>
-    <row r="71" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C71" s="48"/>
-      <c r="D71" s="66"/>
-      <c r="E71" s="66"/>
-      <c r="H71" s="42"/>
-      <c r="I71" s="38"/>
-      <c r="J71" s="39"/>
-      <c r="M71" s="73"/>
+      <c r="O70" s="47"/>
+    </row>
+    <row r="71" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C71" s="52"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="H71" s="56"/>
+      <c r="I71" s="35"/>
+      <c r="J71" s="57"/>
+      <c r="M71" s="46"/>
       <c r="N71" s="10"/>
-      <c r="O71" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="72" spans="3:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C72" s="48"/>
+      <c r="O71" s="48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="72" spans="3:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C72" s="52"/>
       <c r="D72" s="15" t="s">
         <v>92</v>
       </c>
       <c r="E72" s="11"/>
-      <c r="H72" s="42"/>
-      <c r="I72" s="38"/>
-      <c r="J72" s="39"/>
-      <c r="M72" s="73"/>
+      <c r="H72" s="56"/>
+      <c r="I72" s="35"/>
+      <c r="J72" s="57"/>
+      <c r="M72" s="46"/>
       <c r="N72" s="10"/>
-      <c r="O72" s="32"/>
-    </row>
-    <row r="73" spans="3:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C73" s="48"/>
-      <c r="D73" s="29"/>
-      <c r="E73" s="29" t="s">
+      <c r="O72" s="48"/>
+    </row>
+    <row r="73" spans="3:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C73" s="52"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="H73" s="42"/>
+      <c r="H73" s="56"/>
       <c r="I73" s="4"/>
       <c r="J73" s="21"/>
-      <c r="M73" s="73"/>
+      <c r="M73" s="46"/>
       <c r="N73" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="O73" s="10"/>
     </row>
-    <row r="74" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C74" s="48"/>
-      <c r="D74" s="66"/>
-      <c r="E74" s="66"/>
+    <row r="74" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C74" s="52"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
       <c r="H74" s="26"/>
       <c r="I74" s="27"/>
       <c r="J74" s="25"/>
-      <c r="M74" s="73"/>
+      <c r="M74" s="46"/>
       <c r="N74" s="10"/>
       <c r="O74" s="24" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="75" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C75" s="48"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C75" s="52"/>
       <c r="D75" s="15" t="s">
         <v>94</v>
       </c>
@@ -2363,14 +2348,14 @@
       <c r="H75" s="26"/>
       <c r="I75" s="27"/>
       <c r="J75" s="25"/>
-      <c r="M75" s="73"/>
+      <c r="M75" s="46"/>
       <c r="N75" s="10"/>
       <c r="O75" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="76" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="48"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="76" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C76" s="52"/>
       <c r="D76" s="15"/>
       <c r="E76" s="14" t="s">
         <v>95</v>
@@ -2378,60 +2363,60 @@
       <c r="H76" s="26"/>
       <c r="I76" s="28"/>
       <c r="J76" s="27"/>
-      <c r="M76" s="74" t="s">
-        <v>137</v>
-      </c>
-      <c r="N76" s="40"/>
-      <c r="O76" s="49" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="77" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C77" s="48"/>
+      <c r="M76" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="N76" s="50"/>
+      <c r="O76" s="47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C77" s="52"/>
       <c r="D77" s="15"/>
-      <c r="E77" s="49" t="s">
+      <c r="E77" s="47" t="s">
         <v>96</v>
       </c>
       <c r="H77" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I77" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="J77" s="52"/>
-      <c r="M77" s="74"/>
-      <c r="N77" s="41"/>
-      <c r="O77" s="49"/>
-    </row>
-    <row r="78" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="48"/>
+      <c r="I77" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="J77" s="32"/>
+      <c r="M77" s="49"/>
+      <c r="N77" s="51"/>
+      <c r="O77" s="47"/>
+    </row>
+    <row r="78" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C78" s="52"/>
       <c r="D78" s="15"/>
-      <c r="E78" s="49"/>
+      <c r="E78" s="47"/>
       <c r="H78" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I78" s="52" t="s">
+      <c r="I78" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="J78" s="52"/>
-    </row>
-    <row r="79" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="48"/>
+      <c r="J78" s="32"/>
+    </row>
+    <row r="79" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C79" s="52"/>
       <c r="D79" s="15"/>
-      <c r="E79" s="49"/>
+      <c r="E79" s="47"/>
       <c r="H79" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I79" s="52"/>
-      <c r="J79" s="52"/>
-    </row>
-    <row r="80" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="48"/>
-      <c r="D80" s="49" t="s">
+      <c r="I79" s="32"/>
+      <c r="J79" s="32"/>
+    </row>
+    <row r="80" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C80" s="52"/>
+      <c r="D80" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E80" s="50"/>
-      <c r="H80" s="48" t="s">
+      <c r="E80" s="79"/>
+      <c r="H80" s="52" t="s">
         <v>10</v>
       </c>
       <c r="I80" s="2" t="s">
@@ -2442,71 +2427,71 @@
       </c>
       <c r="M80" s="16"/>
     </row>
-    <row r="81" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C81" s="48"/>
-      <c r="D81" s="49"/>
-      <c r="E81" s="51"/>
-      <c r="H81" s="48"/>
-      <c r="I81" s="67" t="s">
-        <v>157</v>
-      </c>
-      <c r="J81" s="38"/>
+    <row r="81" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C81" s="52"/>
+      <c r="D81" s="47"/>
+      <c r="E81" s="80"/>
+      <c r="H81" s="52"/>
+      <c r="I81" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="J81" s="35"/>
       <c r="M81" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N81" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="O81" s="52"/>
-    </row>
-    <row r="82" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C82" s="48"/>
+      <c r="N81" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="O81" s="32"/>
+    </row>
+    <row r="82" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C82" s="52"/>
       <c r="D82" s="11" t="s">
         <v>98</v>
       </c>
       <c r="E82" s="11"/>
-      <c r="H82" s="48"/>
-      <c r="I82" s="69"/>
-      <c r="J82" s="38"/>
+      <c r="H82" s="52"/>
+      <c r="I82" s="43"/>
+      <c r="J82" s="35"/>
       <c r="M82" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N82" s="52" t="s">
+      <c r="N82" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="O82" s="52"/>
-    </row>
-    <row r="83" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C83" s="48"/>
+      <c r="O82" s="32"/>
+    </row>
+    <row r="83" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C83" s="52"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="H83" s="48"/>
+      <c r="H83" s="52"/>
       <c r="I83" s="13"/>
       <c r="J83" s="23" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="M83" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N83" s="52" t="s">
-        <v>149</v>
-      </c>
-      <c r="O83" s="52"/>
-    </row>
-    <row r="84" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C84" s="48"/>
+      <c r="N83" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="O83" s="32"/>
+    </row>
+    <row r="84" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C84" s="52"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H84" s="48"/>
+      <c r="H84" s="52"/>
       <c r="I84" s="13"/>
-      <c r="J84" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="M84" s="48" t="s">
+      <c r="J84" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="M84" s="52" t="s">
         <v>10</v>
       </c>
       <c r="N84" s="2" t="s">
@@ -2516,107 +2501,107 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C85" s="48"/>
+    <row r="85" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C85" s="52"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="H85" s="48"/>
+      <c r="H85" s="52"/>
       <c r="I85" s="13"/>
-      <c r="J85" s="38"/>
-      <c r="M85" s="48"/>
+      <c r="J85" s="35"/>
+      <c r="M85" s="52"/>
       <c r="N85" s="13" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="O85" s="13"/>
     </row>
-    <row r="86" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C86" s="48"/>
-      <c r="D86" s="44"/>
-      <c r="E86" s="49" t="s">
+    <row r="86" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C86" s="52"/>
+      <c r="D86" s="75"/>
+      <c r="E86" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="H86" s="48"/>
-      <c r="I86" s="29"/>
-      <c r="J86" s="38"/>
-      <c r="M86" s="48"/>
+      <c r="H86" s="52"/>
+      <c r="I86" s="36"/>
+      <c r="J86" s="35"/>
+      <c r="M86" s="52"/>
       <c r="N86" s="13"/>
       <c r="O86" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="87" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C87" s="52"/>
+      <c r="D87" s="76"/>
+      <c r="E87" s="47"/>
+      <c r="H87" s="52"/>
+      <c r="I87" s="54"/>
+      <c r="J87" s="35"/>
+      <c r="M87" s="52"/>
+      <c r="N87" s="13"/>
+      <c r="O87" s="47" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="87" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="48"/>
-      <c r="D87" s="45"/>
-      <c r="E87" s="49"/>
-      <c r="H87" s="48"/>
-      <c r="I87" s="30"/>
-      <c r="J87" s="38"/>
-      <c r="M87" s="48"/>
-      <c r="N87" s="13"/>
-      <c r="O87" s="49" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="88" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C88" s="48"/>
+    <row r="88" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C88" s="52"/>
       <c r="D88" s="11" t="s">
         <v>113</v>
       </c>
       <c r="E88" s="11"/>
-      <c r="H88" s="48"/>
-      <c r="I88" s="30"/>
-      <c r="J88" s="38"/>
-      <c r="M88" s="48"/>
+      <c r="H88" s="52"/>
+      <c r="I88" s="54"/>
+      <c r="J88" s="35"/>
+      <c r="M88" s="52"/>
       <c r="N88" s="13"/>
-      <c r="O88" s="49"/>
-    </row>
-    <row r="89" spans="3:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C89" s="48"/>
+      <c r="O88" s="47"/>
+    </row>
+    <row r="89" spans="3:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C89" s="52"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="H89" s="53" t="s">
-        <v>160</v>
-      </c>
-      <c r="I89" s="70"/>
-      <c r="J89" s="38" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="90" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C90" s="42" t="s">
+      <c r="H89" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="I89" s="44"/>
+      <c r="J89" s="35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="90" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C90" s="56" t="s">
         <v>110</v>
       </c>
       <c r="D90" s="20"/>
       <c r="E90" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="H90" s="53"/>
-      <c r="I90" s="71"/>
-      <c r="J90" s="38"/>
-    </row>
-    <row r="91" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C91" s="42"/>
+      <c r="H90" s="41"/>
+      <c r="I90" s="45"/>
+      <c r="J90" s="35"/>
+    </row>
+    <row r="91" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C91" s="56"/>
       <c r="D91" s="20"/>
       <c r="E91" s="21" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C92" s="42"/>
+    <row r="92" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C92" s="56"/>
       <c r="D92" s="20"/>
       <c r="E92" s="21"/>
     </row>
-    <row r="93" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C93" s="42"/>
+    <row r="93" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C93" s="56"/>
       <c r="D93" s="20"/>
       <c r="E93" s="21"/>
     </row>
-    <row r="94" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C94" s="42" t="s">
+    <row r="94" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C94" s="56" t="s">
         <v>102</v>
       </c>
       <c r="D94" s="20"/>
@@ -2626,13 +2611,13 @@
       <c r="H94" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I94" s="52" t="s">
-        <v>162</v>
-      </c>
-      <c r="J94" s="52"/>
-    </row>
-    <row r="95" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C95" s="42"/>
+      <c r="I94" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="J94" s="32"/>
+    </row>
+    <row r="95" spans="3:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="C95" s="56"/>
       <c r="D95" s="20"/>
       <c r="E95" s="21" t="s">
         <v>109</v>
@@ -2640,28 +2625,28 @@
       <c r="H95" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I95" s="52" t="s">
-        <v>170</v>
-      </c>
-      <c r="J95" s="52"/>
-    </row>
-    <row r="96" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C96" s="42"/>
+      <c r="I95" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="J95" s="32"/>
+    </row>
+    <row r="96" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C96" s="56"/>
       <c r="D96" s="20"/>
       <c r="E96" s="21"/>
       <c r="H96" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I96" s="52" t="s">
-        <v>163</v>
-      </c>
-      <c r="J96" s="52"/>
-    </row>
-    <row r="97" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C97" s="42"/>
+      <c r="I96" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="J96" s="32"/>
+    </row>
+    <row r="97" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C97" s="56"/>
       <c r="D97" s="20"/>
       <c r="E97" s="21"/>
-      <c r="H97" s="63" t="s">
+      <c r="H97" s="38" t="s">
         <v>10</v>
       </c>
       <c r="I97" s="2" t="s">
@@ -2671,216 +2656,268 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C98" s="43" t="s">
+    <row r="98" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C98" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="D98" s="44"/>
-      <c r="E98" s="46" t="s">
+      <c r="D98" s="75"/>
+      <c r="E98" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="H98" s="72"/>
-      <c r="I98" s="75" t="s">
-        <v>164</v>
-      </c>
-      <c r="J98" s="38"/>
-    </row>
-    <row r="99" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C99" s="43"/>
-      <c r="D99" s="45"/>
-      <c r="E99" s="47"/>
-      <c r="H99" s="72"/>
-      <c r="I99" s="76"/>
-      <c r="J99" s="38"/>
-    </row>
-    <row r="100" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C100" s="43"/>
+      <c r="H98" s="39"/>
+      <c r="I98" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="J98" s="35"/>
+    </row>
+    <row r="99" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C99" s="74"/>
+      <c r="D99" s="76"/>
+      <c r="E99" s="78"/>
+      <c r="H99" s="39"/>
+      <c r="I99" s="34"/>
+      <c r="J99" s="35"/>
+    </row>
+    <row r="100" spans="3:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="C100" s="74"/>
       <c r="D100" s="20"/>
       <c r="E100" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="H100" s="72"/>
+      <c r="H100" s="39"/>
       <c r="I100" s="13"/>
-      <c r="J100" s="29" t="s">
-        <v>165</v>
+      <c r="J100" s="36" t="s">
+        <v>162</v>
       </c>
       <c r="M100" s="16"/>
     </row>
-    <row r="101" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C101" s="43"/>
+    <row r="101" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C101" s="74"/>
       <c r="D101" s="20"/>
       <c r="E101" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="H101" s="72"/>
+      <c r="H101" s="39"/>
       <c r="I101" s="13"/>
-      <c r="J101" s="66"/>
-    </row>
-    <row r="102" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C102" s="35" t="s">
+      <c r="J101" s="37"/>
+    </row>
+    <row r="102" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C102" s="71" t="s">
         <v>115</v>
       </c>
       <c r="D102" s="20"/>
       <c r="E102" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="H102" s="72"/>
+      <c r="H102" s="39"/>
       <c r="I102" s="13"/>
-      <c r="J102" s="29" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="103" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C103" s="36"/>
+      <c r="J102" s="36" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="103" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C103" s="72"/>
       <c r="D103" s="20"/>
       <c r="E103" s="22"/>
-      <c r="H103" s="72"/>
+      <c r="H103" s="39"/>
       <c r="I103" s="23"/>
-      <c r="J103" s="66"/>
-    </row>
-    <row r="104" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C104" s="37"/>
+      <c r="J103" s="37"/>
+    </row>
+    <row r="104" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C104" s="73"/>
       <c r="D104" s="20"/>
       <c r="E104" s="21"/>
-      <c r="H104" s="77"/>
+      <c r="H104" s="40"/>
       <c r="I104" s="23"/>
-      <c r="J104" s="23" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="105" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C105" s="35" t="s">
+      <c r="J104" s="23"/>
+    </row>
+    <row r="105" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C105" s="72"/>
+      <c r="D105" s="30"/>
+      <c r="E105" s="29"/>
+      <c r="H105" s="26"/>
+      <c r="I105" s="27"/>
+      <c r="J105" s="27"/>
+    </row>
+    <row r="106" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C106" s="72"/>
+      <c r="D106" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E106" s="10"/>
+      <c r="H106" s="26"/>
+      <c r="I106" s="27"/>
+      <c r="J106" s="27"/>
+    </row>
+    <row r="107" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C107" s="73"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H107" s="26"/>
+      <c r="I107" s="27"/>
+      <c r="J107" s="27"/>
+    </row>
+    <row r="108" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C108" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="D108" s="13"/>
+      <c r="E108" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="D105" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="E105" s="39"/>
-      <c r="H105" s="53" t="s">
-        <v>168</v>
-      </c>
-      <c r="I105" s="38"/>
-      <c r="J105" s="38" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="106" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C106" s="36"/>
-      <c r="D106" s="38"/>
-      <c r="E106" s="39"/>
-      <c r="H106" s="53"/>
-      <c r="I106" s="38"/>
-      <c r="J106" s="38"/>
-    </row>
-    <row r="107" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C107" s="36"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="H107" s="53"/>
-      <c r="I107" s="38"/>
-      <c r="J107" s="38"/>
-    </row>
-    <row r="108" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C108" s="36"/>
-      <c r="D108" s="40"/>
-      <c r="E108" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="H108" s="53"/>
-      <c r="I108" s="10"/>
-      <c r="J108" s="10"/>
-    </row>
-    <row r="109" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C109" s="36"/>
-      <c r="D109" s="41"/>
-      <c r="E109" s="32"/>
-      <c r="H109" s="26"/>
-      <c r="I109" s="27"/>
-      <c r="J109" s="27"/>
-    </row>
-    <row r="110" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C110" s="36"/>
-      <c r="D110" s="10" t="s">
+      <c r="H108" s="26"/>
+      <c r="I108" s="31"/>
+      <c r="J108" s="31"/>
+    </row>
+    <row r="109" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C109" s="62"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="48"/>
+    </row>
+    <row r="110" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C110" s="62"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="111" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C111" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E110" s="10"/>
-      <c r="H110" s="26"/>
-      <c r="I110" s="27"/>
-      <c r="J110" s="27"/>
-    </row>
-    <row r="111" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C111" s="37"/>
-      <c r="D111" s="10"/>
-      <c r="E111" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="H111" s="26"/>
-      <c r="I111" s="27"/>
-      <c r="J111" s="27"/>
-    </row>
-    <row r="112" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C112" s="31" t="s">
-        <v>123</v>
-      </c>
+    </row>
+    <row r="112" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C112" s="70"/>
       <c r="D112" s="13"/>
-      <c r="E112" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="H112" s="26"/>
-      <c r="I112" s="78"/>
-      <c r="J112" s="78"/>
-    </row>
-    <row r="113" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C113" s="31"/>
+      <c r="E112" s="13"/>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C113" s="70"/>
       <c r="D113" s="13"/>
-      <c r="E113" s="32"/>
-    </row>
-    <row r="114" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C114" s="31"/>
-      <c r="D114" s="13"/>
-      <c r="E114" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="115" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C115" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="D115" s="13"/>
-      <c r="E115" s="13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C116" s="34"/>
-      <c r="D116" s="13"/>
-      <c r="E116" s="13"/>
-    </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C117" s="34"/>
-      <c r="D117" s="13"/>
-      <c r="E117" s="13"/>
-    </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C118" s="34"/>
-      <c r="D118" s="10"/>
-      <c r="E118" s="10"/>
+      <c r="E113" s="13"/>
+    </row>
+    <row r="114" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C114" s="70"/>
+      <c r="D114" s="10"/>
+      <c r="E114" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="148">
-    <mergeCell ref="I94:J94"/>
-    <mergeCell ref="I95:J95"/>
-    <mergeCell ref="I96:J96"/>
-    <mergeCell ref="I98:I99"/>
-    <mergeCell ref="J98:J99"/>
-    <mergeCell ref="J100:J101"/>
-    <mergeCell ref="J102:J103"/>
-    <mergeCell ref="H97:H104"/>
-    <mergeCell ref="H105:H108"/>
-    <mergeCell ref="J105:J107"/>
-    <mergeCell ref="I105:I107"/>
+  <mergeCells count="141">
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="H89:H90"/>
+    <mergeCell ref="H80:H88"/>
+    <mergeCell ref="C94:C97"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="C69:C89"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="E77:E79"/>
+    <mergeCell ref="C108:C110"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="C111:C114"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="C105:C107"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="H7:H13"/>
+    <mergeCell ref="M7:M19"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="N10:N12"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M20:M24"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="H23:H27"/>
+    <mergeCell ref="M25:M29"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="H28:H32"/>
+    <mergeCell ref="I28:I32"/>
+    <mergeCell ref="J28:J32"/>
+    <mergeCell ref="M30:M34"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="D42:D46"/>
+    <mergeCell ref="E42:E46"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="H46:H50"/>
+    <mergeCell ref="M46:M49"/>
+    <mergeCell ref="M50:M52"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="M53:M55"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="M56:M57"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="H61:H69"/>
+    <mergeCell ref="J62:J65"/>
+    <mergeCell ref="I67:I69"/>
+    <mergeCell ref="J67:J69"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="I70:I72"/>
+    <mergeCell ref="J70:J72"/>
     <mergeCell ref="I81:I82"/>
     <mergeCell ref="J81:J82"/>
     <mergeCell ref="I89:I90"/>
@@ -2904,120 +2941,15 @@
     <mergeCell ref="I78:J78"/>
     <mergeCell ref="I79:J79"/>
     <mergeCell ref="J84:J88"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="H61:H69"/>
-    <mergeCell ref="J62:J65"/>
-    <mergeCell ref="I67:I69"/>
-    <mergeCell ref="J67:J69"/>
-    <mergeCell ref="H70:H73"/>
-    <mergeCell ref="I70:I72"/>
-    <mergeCell ref="J70:J72"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="C37:C41"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="D42:D46"/>
-    <mergeCell ref="E42:E46"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="H46:H50"/>
-    <mergeCell ref="M46:M49"/>
-    <mergeCell ref="M50:M52"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="M53:M55"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="M56:M57"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="M25:M29"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="H28:H32"/>
-    <mergeCell ref="I28:I32"/>
-    <mergeCell ref="J28:J32"/>
-    <mergeCell ref="M30:M34"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="O30:O32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M20:M24"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="H7:H13"/>
-    <mergeCell ref="M7:M19"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="N10:N12"/>
-    <mergeCell ref="O10:O12"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="N6:O6"/>
     <mergeCell ref="I86:I88"/>
-    <mergeCell ref="C112:C114"/>
-    <mergeCell ref="E112:E113"/>
-    <mergeCell ref="C115:C118"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="C105:C111"/>
-    <mergeCell ref="C94:C97"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="C69:C89"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="E77:E79"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="H89:H90"/>
-    <mergeCell ref="H80:H88"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="I95:J95"/>
+    <mergeCell ref="I96:J96"/>
+    <mergeCell ref="I98:I99"/>
+    <mergeCell ref="J98:J99"/>
+    <mergeCell ref="J100:J101"/>
+    <mergeCell ref="J102:J103"/>
+    <mergeCell ref="H97:H104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>